<commit_message>
organizing the lock mechanism in ExcelPrinter
</commit_message>
<xml_diff>
--- a/output/result.xlsx
+++ b/output/result.xlsx
@@ -62,7 +62,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -189,11 +189,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00CCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00CCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00CCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="00CCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00CCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="00CCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00CCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="00CCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00CCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="00CCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="00CCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -213,6 +277,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>

</xml_diff>

<commit_message>
a colocar tudo no mesmo excel
</commit_message>
<xml_diff>
--- a/output/result.xlsx
+++ b/output/result.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="VPE" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="RH" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Avaliacao-Vice-Presidente-Externo" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Avaliacao-Membro-RH" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -62,7 +62,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -189,75 +189,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="00CCCCCC"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="00CCCCCC"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00CCCCCC"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="00CCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="00CCCCCC"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="00CCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00CCCCCC"/>
-      </left>
-      <right style="thin">
-        <color rgb="00CCCCCC"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00CCCCCC"/>
-      </left>
-      <right style="thin">
-        <color rgb="00CCCCCC"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="00CCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -277,13 +213,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>

</xml_diff>

<commit_message>
adicionei mais locks aos logs...
</commit_message>
<xml_diff>
--- a/output/result.xlsx
+++ b/output/result.xlsx
@@ -1726,7 +1726,7 @@
       <c r="A4" s="7" t="n"/>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Goncalo Figueiredo</t>
         </is>
       </c>
       <c r="D4" s="7" t="n"/>
@@ -1793,7 +1793,7 @@
       <c r="A5" s="7" t="n"/>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>Inês Cabral</t>
+          <t>Ines Cabral</t>
         </is>
       </c>
       <c r="D5" s="7" t="n"/>
@@ -2271,7 +2271,7 @@
       <c r="A12" s="7" t="n"/>
       <c r="C12" s="5" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Goncalo Figueiredo</t>
         </is>
       </c>
       <c r="D12" s="7" t="n"/>
@@ -2338,7 +2338,7 @@
       <c r="A13" s="7" t="n"/>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>Inês Cabral</t>
+          <t>Ines Cabral</t>
         </is>
       </c>
       <c r="D13" s="7" t="n"/>
@@ -2816,7 +2816,7 @@
       <c r="A20" s="7" t="n"/>
       <c r="C20" s="5" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Goncalo Figueiredo</t>
         </is>
       </c>
       <c r="D20" s="7" t="n"/>
@@ -2883,7 +2883,7 @@
       <c r="A21" s="7" t="n"/>
       <c r="C21" s="5" t="inlineStr">
         <is>
-          <t>Inês Cabral</t>
+          <t>Ines Cabral</t>
         </is>
       </c>
       <c r="D21" s="7" t="n"/>
@@ -3361,7 +3361,7 @@
       <c r="A28" s="7" t="n"/>
       <c r="C28" s="5" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Goncalo Figueiredo</t>
         </is>
       </c>
       <c r="D28" s="7" t="n"/>
@@ -3428,7 +3428,7 @@
       <c r="A29" s="7" t="n"/>
       <c r="C29" s="5" t="inlineStr">
         <is>
-          <t>Inês Cabral</t>
+          <t>Ines Cabral</t>
         </is>
       </c>
       <c r="D29" s="7" t="n"/>
@@ -3906,7 +3906,7 @@
       <c r="A36" s="7" t="n"/>
       <c r="C36" s="5" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Goncalo Figueiredo</t>
         </is>
       </c>
       <c r="D36" s="7" t="n"/>
@@ -3973,7 +3973,7 @@
       <c r="A37" s="7" t="n"/>
       <c r="C37" s="5" t="inlineStr">
         <is>
-          <t>Inês Cabral</t>
+          <t>Ines Cabral</t>
         </is>
       </c>
       <c r="D37" s="7" t="n"/>
@@ -4451,7 +4451,7 @@
       <c r="A44" s="7" t="n"/>
       <c r="C44" s="5" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Goncalo Figueiredo</t>
         </is>
       </c>
       <c r="D44" s="7" t="n"/>
@@ -4518,7 +4518,7 @@
       <c r="A45" s="7" t="n"/>
       <c r="C45" s="5" t="inlineStr">
         <is>
-          <t>Inês Cabral</t>
+          <t>Ines Cabral</t>
         </is>
       </c>
       <c r="D45" s="7" t="n"/>
@@ -4996,7 +4996,7 @@
       <c r="A52" s="7" t="n"/>
       <c r="C52" s="5" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Goncalo Figueiredo</t>
         </is>
       </c>
       <c r="D52" s="7" t="n"/>
@@ -5063,7 +5063,7 @@
       <c r="A53" s="7" t="n"/>
       <c r="C53" s="5" t="inlineStr">
         <is>
-          <t>Inês Cabral</t>
+          <t>Ines Cabral</t>
         </is>
       </c>
       <c r="D53" s="7" t="n"/>
@@ -5541,7 +5541,7 @@
       <c r="A60" s="7" t="n"/>
       <c r="C60" s="5" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Goncalo Figueiredo</t>
         </is>
       </c>
       <c r="D60" s="7" t="n"/>
@@ -5608,7 +5608,7 @@
       <c r="A61" s="7" t="n"/>
       <c r="C61" s="5" t="inlineStr">
         <is>
-          <t>Inês Cabral</t>
+          <t>Ines Cabral</t>
         </is>
       </c>
       <c r="D61" s="7" t="n"/>
@@ -6086,7 +6086,7 @@
       <c r="A68" s="7" t="n"/>
       <c r="C68" s="5" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Goncalo Figueiredo</t>
         </is>
       </c>
       <c r="D68" s="7" t="n"/>
@@ -6153,7 +6153,7 @@
       <c r="A69" s="7" t="n"/>
       <c r="C69" s="5" t="inlineStr">
         <is>
-          <t>Inês Cabral</t>
+          <t>Ines Cabral</t>
         </is>
       </c>
       <c r="D69" s="7" t="n"/>

</xml_diff>

<commit_message>
omenos ja aparecem coisas no excel
</commit_message>
<xml_diff>
--- a/output/result.xlsx
+++ b/output/result.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Avaliacao-Membros-MKT" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Avaliacao-Membro-RH" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Avaliacao" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="resultado" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -36,7 +37,7 @@
       <color rgb="00000000"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -61,6 +62,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00DDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ffffff"/>
       </patternFill>
     </fill>
   </fills>
@@ -323,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -366,6 +372,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -15268,7 +15277,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="B1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15279,140 +15288,140 @@
     <row r="1">
       <c r="B1" t="inlineStr">
         <is>
-          <t>Pedro Machado</t>
+          <t>Catarina Milheiro</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="B2" t="inlineStr">
         <is>
-          <t>Beatriz Simoes</t>
+          <t>Goncalo Figueiredo</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
-          <t>Beatriz Sousa</t>
+          <t>Ines Cabral</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>Catarina Oliveira</t>
+          <t>Mariana Arezes</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>Claudia Santos</t>
+          <t>Mariana Oliveira</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ines Faria</t>
+          <t>Paula Ferreira</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ines Geraldes</t>
+          <t>Paulo Vieira</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="inlineStr">
         <is>
-          <t>Leticia Santos</t>
+          <t>Rafaela Carvalho</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="inlineStr">
         <is>
-          <t>Marcia Costa</t>
+          <t>Pedro Machado</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="inlineStr">
         <is>
-          <t>Margarida Ribeiro</t>
+          <t>Beatriz Simoes</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="inlineStr">
         <is>
-          <t>Mariana Coelho</t>
+          <t>Beatriz Sousa</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="inlineStr">
         <is>
-          <t>Raquel Baptista</t>
+          <t>Catarina Oliveira</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="inlineStr">
         <is>
-          <t>Catarina Milheiro</t>
+          <t>Claudia Santos</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="inlineStr">
         <is>
-          <t>Goncalo Figueiredo</t>
+          <t>Ines Faria</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="inlineStr">
         <is>
-          <t>Ines Cabral</t>
+          <t>Ines Geraldes</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="inlineStr">
         <is>
-          <t>Mariana Arezes</t>
+          <t>Leticia Santos</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="inlineStr">
         <is>
-          <t>Mariana Oliveira</t>
+          <t>Marcia Costa</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="inlineStr">
         <is>
-          <t>Paula Ferreira</t>
+          <t>Margarida Ribeiro</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="inlineStr">
         <is>
-          <t>Paulo Vieira</t>
+          <t>Mariana Coelho</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="inlineStr">
         <is>
-          <t>Rafaela Carvalho</t>
+          <t>Raquel Baptista</t>
         </is>
       </c>
     </row>
@@ -15424,4 +15433,149 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),)</f>
+        <v/>
+      </c>
+      <c r="B1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 2, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 4, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <v/>
+      </c>
+      <c r="C1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 2, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 4, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <v/>
+      </c>
+      <c r="D1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 2, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <v/>
+      </c>
+      <c r="E1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 2, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),)</f>
+        <v/>
+      </c>
+      <c r="F1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 2, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 3, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 4, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 4, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <v/>
+      </c>
+      <c r="G1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 2, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <v/>
+      </c>
+      <c r="H1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 4, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 3, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),)</f>
+        <v/>
+      </c>
+      <c r="I1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 2, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 4, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <v/>
+      </c>
+      <c r="J1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),)</f>
+        <v/>
+      </c>
+      <c r="K1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),)</f>
+        <v/>
+      </c>
+      <c r="L1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 2, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 4, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 4, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 4, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 3, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <v/>
+      </c>
+      <c r="M1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),)</f>
+        <v/>
+      </c>
+      <c r="N1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),)</f>
+        <v/>
+      </c>
+      <c r="O1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <v/>
+      </c>
+      <c r="P1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <v/>
+      </c>
+      <c r="Q1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <v/>
+      </c>
+      <c r="R1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 4, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <v/>
+      </c>
+      <c r="S1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 2, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),)</f>
+        <v/>
+      </c>
+      <c r="T1" s="28">
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais., ""),SE(Avaliacao!A1="Goncalo Figueiredo", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais., ""),SE(Avaliacao!A1="Ines Cabral", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais., ""),SE(Avaliacao!A1="Mariana Arezes", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais., ""),SE(Avaliacao!A1="Mariana Oliveira", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais., ""),SE(Avaliacao!A1="Paula Ferreira", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais., ""),SE(Avaliacao!A1="Paulo Vieira", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais., ""),SE(Avaliacao!A1="Rafaela Carvalho", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais., ""),SE(Avaliacao!A1="Catarina Milheiro", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais, ""),SE(Avaliacao!A1="Goncalo Figueiredo", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais, ""),SE(Avaliacao!A1="Ines Cabral", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais, ""),SE(Avaliacao!A1="Mariana Arezes", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais, ""),SE(Avaliacao!A1="Mariana Oliveira", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais, ""),SE(Avaliacao!A1="Paula Ferreira", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais, ""),SE(Avaliacao!A1="Paulo Vieira", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais, ""),SE(Avaliacao!A1="Rafaela Carvalho", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais, ""),SE(Avaliacao!A1="Catarina Milheiro", Nada a apontar, ""),SE(Avaliacao!A1="Goncalo Figueiredo", Nada a apontar, ""),SE(Avaliacao!A1="Ines Cabral", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Arezes", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Oliveira", Nada a apontar, ""),SE(Avaliacao!A1="Paula Ferreira", Nada a apontar, ""),SE(Avaliacao!A1="Paulo Vieira", Nada a apontar, ""),SE(Avaliacao!A1="Rafaela Carvalho", Nada a apontar, ""),SE(Avaliacao!A1="Catarina Milheiro", Nada a apontar, ""),SE(Avaliacao!A1="Goncalo Figueiredo", Nada a apontar, ""),SE(Avaliacao!A1="Ines Cabral", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Arezes", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Oliveira", Nada a apontar, ""),SE(Avaliacao!A1="Paula Ferreira", Nada a apontar, ""),SE(Avaliacao!A1="Paulo Vieira", Nada a apontar, ""),SE(Avaliacao!A1="Rafaela Carvalho", Nada a apontar, ""),SE(Avaliacao!A1="Catarina Milheiro", Nada a apontar, ""),SE(Avaliacao!A1="Goncalo Figueiredo", Nada a apontar, ""),SE(Avaliacao!A1="Ines Cabral", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Arezes", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Oliveira", Nada a apontar, ""),SE(Avaliacao!A1="Paula Ferreira", Nada a apontar, ""),SE(Avaliacao!A1="Paulo Vieira", Nada a apontar, ""),SE(Avaliacao!A1="Rafaela Carvalho", Nada a apontar, ""),SE(Avaliacao!A1="Catarina Milheiro", Nada a apontar, ""),SE(Avaliacao!A1="Goncalo Figueiredo", Nada a apontar, ""),SE(Avaliacao!A1="Ines Cabral", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Arezes", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Oliveira", Nada a apontar, ""),SE(Avaliacao!A1="Paula Ferreira", Nada a apontar, ""),SE(Avaliacao!A1="Paulo Vieira", Nada a apontar, ""),SE(Avaliacao!A1="Rafaela Carvalho", Nada a apontar, ""),SE(Avaliacao!A1="Catarina Milheiro", Nada a apontar, ""),SE(Avaliacao!A1="Goncalo Figueiredo", Nada a apontar, ""),SE(Avaliacao!A1="Ines Cabral", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Arezes", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Oliveira", Nada a apontar, ""),SE(Avaliacao!A1="Paula Ferreira", Nada a apontar, ""),SE(Avaliacao!A1="Paulo Vieira", Nada a apontar, ""),SE(Avaliacao!A1="Rafaela Carvalho", Nada a apontar, ""),SE(Avaliacao!A1="Catarina Milheiro", Nada a apontar, ""),SE(Avaliacao!A1="Goncalo Figueiredo", Nada a apontar, ""),SE(Avaliacao!A1="Ines Cabral", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Arezes", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Oliveira", Nada a apontar, ""),SE(Avaliacao!A1="Paula Ferreira", Nada a apontar, ""),SE(Avaliacao!A1="Paulo Vieira", Nada a apontar, ""),SE(Avaliacao!A1="Rafaela Carvalho", Nada a apontar, ""),SE(Avaliacao!A1="Catarina Milheiro", Nada a apontar, ""),SE(Avaliacao!A1="Goncalo Figueiredo", Nada a apontar, ""),SE(Avaliacao!A1="Ines Cabral", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Arezes", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Oliveira", Nada a apontar, ""),SE(Avaliacao!A1="Paula Ferreira", Nada a apontar, ""),SE(Avaliacao!A1="Paulo Vieira", Nada a apontar, ""),SE(Avaliacao!A1="Rafaela Carvalho", Nada a apontar, ""),)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n"/>
+      <c r="B2" s="4" t="n"/>
+      <c r="C2" s="4" t="n"/>
+      <c r="D2" s="4" t="n"/>
+      <c r="E2" s="4" t="n"/>
+      <c r="F2" s="4" t="n"/>
+      <c r="G2" s="4" t="n"/>
+      <c r="H2" s="4" t="n"/>
+      <c r="I2" s="4" t="n"/>
+      <c r="J2" s="4" t="n"/>
+      <c r="K2" s="4" t="n"/>
+      <c r="L2" s="4" t="n"/>
+      <c r="M2" s="4" t="n"/>
+      <c r="N2" s="4" t="n"/>
+      <c r="O2" s="4" t="n"/>
+      <c r="P2" s="4" t="n"/>
+      <c r="Q2" s="4" t="n"/>
+      <c r="R2" s="4" t="n"/>
+      <c r="S2" s="4" t="n"/>
+      <c r="T2" s="4" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="R1:R2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
a fazer aperfeicoamentos aos resultados
</commit_message>
<xml_diff>
--- a/output/result.xlsx
+++ b/output/result.xlsx
@@ -15451,83 +15451,83 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 5.4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4.0, ""),SE(Avaliacao!A1="Ines Cabral", 4.5, ""),SE(Avaliacao!A1="Mariana Arezes", 5.1, ""),SE(Avaliacao!A1="Mariana Oliveira", 5.4, ""),SE(Avaliacao!A1="Paula Ferreira", 5.4, ""),SE(Avaliacao!A1="Paulo Vieira", 4.8, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4.7, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
       <c r="B1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 2, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 4, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 5.3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3.6, ""),SE(Avaliacao!A1="Ines Cabral", 4.3, ""),SE(Avaliacao!A1="Mariana Arezes", 4.9, ""),SE(Avaliacao!A1="Mariana Oliveira", 5.2, ""),SE(Avaliacao!A1="Paula Ferreira", 5.2, ""),SE(Avaliacao!A1="Paulo Vieira", 4.6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4.6, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
       <c r="C1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 2, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 4, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 5.4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3.8, ""),SE(Avaliacao!A1="Ines Cabral", 4.6, ""),SE(Avaliacao!A1="Mariana Arezes", 5.1, ""),SE(Avaliacao!A1="Mariana Oliveira", 5.2, ""),SE(Avaliacao!A1="Paula Ferreira", 5.2, ""),SE(Avaliacao!A1="Paulo Vieira", 4.5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4.8, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
       <c r="D1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 2, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 5.3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4.1, ""),SE(Avaliacao!A1="Ines Cabral", 4.7, ""),SE(Avaliacao!A1="Mariana Arezes", 5.1, ""),SE(Avaliacao!A1="Mariana Oliveira", 5.3, ""),SE(Avaliacao!A1="Paula Ferreira", 5.3, ""),SE(Avaliacao!A1="Paulo Vieira", 4.9, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4.8, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
       <c r="E1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 2, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 5.4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3.5, ""),SE(Avaliacao!A1="Ines Cabral", 4.4, ""),SE(Avaliacao!A1="Mariana Arezes", 5.0, ""),SE(Avaliacao!A1="Mariana Oliveira", 5.3, ""),SE(Avaliacao!A1="Paula Ferreira", 5.1, ""),SE(Avaliacao!A1="Paulo Vieira", 4.3, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4.3, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
       <c r="F1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 2, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 3, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 4, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 4, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 5.3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4.2, ""),SE(Avaliacao!A1="Ines Cabral", 4.5, ""),SE(Avaliacao!A1="Mariana Arezes", 5.0, ""),SE(Avaliacao!A1="Mariana Oliveira", 5.1, ""),SE(Avaliacao!A1="Paula Ferreira", 4.9, ""),SE(Avaliacao!A1="Paulo Vieira", 4.8, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4.7, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
       <c r="G1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 2, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 5.3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4.1, ""),SE(Avaliacao!A1="Ines Cabral", 4.5, ""),SE(Avaliacao!A1="Mariana Arezes", 4.9, ""),SE(Avaliacao!A1="Mariana Oliveira", 5.2, ""),SE(Avaliacao!A1="Paula Ferreira", 5.0, ""),SE(Avaliacao!A1="Paulo Vieira", 4.4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4.7, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
       <c r="H1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 4, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 3, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 5.4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4.1, ""),SE(Avaliacao!A1="Ines Cabral", 4.9, ""),SE(Avaliacao!A1="Mariana Arezes", 5.2, ""),SE(Avaliacao!A1="Mariana Oliveira", 5.3, ""),SE(Avaliacao!A1="Paula Ferreira", 5.2, ""),SE(Avaliacao!A1="Paulo Vieira", 4.5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4.8, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
       <c r="I1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 2, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 4, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 5.4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3.8, ""),SE(Avaliacao!A1="Ines Cabral", 4.6, ""),SE(Avaliacao!A1="Mariana Arezes", 4.9, ""),SE(Avaliacao!A1="Mariana Oliveira", 5.2, ""),SE(Avaliacao!A1="Paula Ferreira", 5.4, ""),SE(Avaliacao!A1="Paulo Vieira", 4.5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4.8, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
       <c r="J1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 4.9, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4.6, ""),SE(Avaliacao!A1="Ines Cabral", 4.9, ""),SE(Avaliacao!A1="Mariana Arezes", 5.3, ""),SE(Avaliacao!A1="Mariana Oliveira", 5.1, ""),SE(Avaliacao!A1="Paula Ferreira", 5.1, ""),SE(Avaliacao!A1="Paulo Vieira", 5.1, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5.0, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
       <c r="K1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 5.4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5.4, ""),SE(Avaliacao!A1="Ines Cabral", 5.3, ""),SE(Avaliacao!A1="Mariana Arezes", 5.4, ""),SE(Avaliacao!A1="Mariana Oliveira", 5.4, ""),SE(Avaliacao!A1="Paula Ferreira", 5.4, ""),SE(Avaliacao!A1="Paulo Vieira", 5.4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5.4, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
       <c r="L1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 2, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 4, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 4, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 4, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 3, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 4, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 4.8, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4.0, ""),SE(Avaliacao!A1="Ines Cabral", 4.2, ""),SE(Avaliacao!A1="Mariana Arezes", 4.7, ""),SE(Avaliacao!A1="Mariana Oliveira", 4.7, ""),SE(Avaliacao!A1="Paula Ferreira", 4.5, ""),SE(Avaliacao!A1="Paulo Vieira", 4.2, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4.3, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
       <c r="M1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 5.4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4.9, ""),SE(Avaliacao!A1="Ines Cabral", 5.0, ""),SE(Avaliacao!A1="Mariana Arezes", 5.3, ""),SE(Avaliacao!A1="Mariana Oliveira", 5.3, ""),SE(Avaliacao!A1="Paula Ferreira", 5.4, ""),SE(Avaliacao!A1="Paulo Vieira", 5.1, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5.1, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
       <c r="N1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 5.4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5.2, ""),SE(Avaliacao!A1="Ines Cabral", 5.3, ""),SE(Avaliacao!A1="Mariana Arezes", 5.4, ""),SE(Avaliacao!A1="Mariana Oliveira", 5.4, ""),SE(Avaliacao!A1="Paula Ferreira", 5.4, ""),SE(Avaliacao!A1="Paulo Vieira", 5.4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5.3, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
       <c r="O1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 5.4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4.3, ""),SE(Avaliacao!A1="Ines Cabral", 4.9, ""),SE(Avaliacao!A1="Mariana Arezes", 5.1, ""),SE(Avaliacao!A1="Mariana Oliveira", 5.3, ""),SE(Avaliacao!A1="Paula Ferreira", 5.4, ""),SE(Avaliacao!A1="Paulo Vieira", 4.8, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4.9, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
       <c r="P1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 5.3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3.9, ""),SE(Avaliacao!A1="Ines Cabral", 4.7, ""),SE(Avaliacao!A1="Mariana Arezes", 4.9, ""),SE(Avaliacao!A1="Mariana Oliveira", 5.2, ""),SE(Avaliacao!A1="Paula Ferreira", 5.3, ""),SE(Avaliacao!A1="Paulo Vieira", 4.7, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4.8, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
       <c r="Q1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paula Ferreira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 5.2, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4.6, ""),SE(Avaliacao!A1="Ines Cabral", 4.7, ""),SE(Avaliacao!A1="Mariana Arezes", 5.0, ""),SE(Avaliacao!A1="Mariana Oliveira", 5.2, ""),SE(Avaliacao!A1="Paula Ferreira", 4.9, ""),SE(Avaliacao!A1="Paulo Vieira", 5.0, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4.7, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
       <c r="R1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 5, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 4, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 5.3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5.0, ""),SE(Avaliacao!A1="Ines Cabral", 4.9, ""),SE(Avaliacao!A1="Mariana Arezes", 5.3, ""),SE(Avaliacao!A1="Mariana Oliveira", 5.4, ""),SE(Avaliacao!A1="Paula Ferreira", 5.2, ""),SE(Avaliacao!A1="Paulo Vieira", 5.2, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5.1, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
       <c r="S1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Catarina Milheiro", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 2, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 5, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 3, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 5, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Ines Cabral", 4, ""),SE(Avaliacao!A1="Ines Cabral", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 5, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Arezes", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 5, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Mariana Oliveira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paula Ferreira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 5, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Paulo Vieira", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 5, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4, ""),SE(Avaliacao!A1="Rafaela Carvalho", 6, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 5.4, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 4.2, ""),SE(Avaliacao!A1="Ines Cabral", 4.6, ""),SE(Avaliacao!A1="Mariana Arezes", 5.2, ""),SE(Avaliacao!A1="Mariana Oliveira", 5.3, ""),SE(Avaliacao!A1="Paula Ferreira", 5.4, ""),SE(Avaliacao!A1="Paulo Vieira", 5.0, ""),SE(Avaliacao!A1="Rafaela Carvalho", 4.7, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
       <c r="T1" s="28">
-        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais., ""),SE(Avaliacao!A1="Goncalo Figueiredo", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais., ""),SE(Avaliacao!A1="Ines Cabral", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais., ""),SE(Avaliacao!A1="Mariana Arezes", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais., ""),SE(Avaliacao!A1="Mariana Oliveira", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais., ""),SE(Avaliacao!A1="Paula Ferreira", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais., ""),SE(Avaliacao!A1="Paulo Vieira", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais., ""),SE(Avaliacao!A1="Rafaela Carvalho", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais., ""),SE(Avaliacao!A1="Catarina Milheiro", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais, ""),SE(Avaliacao!A1="Goncalo Figueiredo", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais, ""),SE(Avaliacao!A1="Ines Cabral", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais, ""),SE(Avaliacao!A1="Mariana Arezes", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais, ""),SE(Avaliacao!A1="Mariana Oliveira", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais, ""),SE(Avaliacao!A1="Paula Ferreira", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais, ""),SE(Avaliacao!A1="Paulo Vieira", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais, ""),SE(Avaliacao!A1="Rafaela Carvalho", Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais, ""),SE(Avaliacao!A1="Catarina Milheiro", Nada a apontar, ""),SE(Avaliacao!A1="Goncalo Figueiredo", Nada a apontar, ""),SE(Avaliacao!A1="Ines Cabral", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Arezes", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Oliveira", Nada a apontar, ""),SE(Avaliacao!A1="Paula Ferreira", Nada a apontar, ""),SE(Avaliacao!A1="Paulo Vieira", Nada a apontar, ""),SE(Avaliacao!A1="Rafaela Carvalho", Nada a apontar, ""),SE(Avaliacao!A1="Catarina Milheiro", Nada a apontar, ""),SE(Avaliacao!A1="Goncalo Figueiredo", Nada a apontar, ""),SE(Avaliacao!A1="Ines Cabral", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Arezes", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Oliveira", Nada a apontar, ""),SE(Avaliacao!A1="Paula Ferreira", Nada a apontar, ""),SE(Avaliacao!A1="Paulo Vieira", Nada a apontar, ""),SE(Avaliacao!A1="Rafaela Carvalho", Nada a apontar, ""),SE(Avaliacao!A1="Catarina Milheiro", Nada a apontar, ""),SE(Avaliacao!A1="Goncalo Figueiredo", Nada a apontar, ""),SE(Avaliacao!A1="Ines Cabral", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Arezes", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Oliveira", Nada a apontar, ""),SE(Avaliacao!A1="Paula Ferreira", Nada a apontar, ""),SE(Avaliacao!A1="Paulo Vieira", Nada a apontar, ""),SE(Avaliacao!A1="Rafaela Carvalho", Nada a apontar, ""),SE(Avaliacao!A1="Catarina Milheiro", Nada a apontar, ""),SE(Avaliacao!A1="Goncalo Figueiredo", Nada a apontar, ""),SE(Avaliacao!A1="Ines Cabral", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Arezes", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Oliveira", Nada a apontar, ""),SE(Avaliacao!A1="Paula Ferreira", Nada a apontar, ""),SE(Avaliacao!A1="Paulo Vieira", Nada a apontar, ""),SE(Avaliacao!A1="Rafaela Carvalho", Nada a apontar, ""),SE(Avaliacao!A1="Catarina Milheiro", Nada a apontar, ""),SE(Avaliacao!A1="Goncalo Figueiredo", Nada a apontar, ""),SE(Avaliacao!A1="Ines Cabral", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Arezes", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Oliveira", Nada a apontar, ""),SE(Avaliacao!A1="Paula Ferreira", Nada a apontar, ""),SE(Avaliacao!A1="Paulo Vieira", Nada a apontar, ""),SE(Avaliacao!A1="Rafaela Carvalho", Nada a apontar, ""),SE(Avaliacao!A1="Catarina Milheiro", Nada a apontar, ""),SE(Avaliacao!A1="Goncalo Figueiredo", Nada a apontar, ""),SE(Avaliacao!A1="Ines Cabral", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Arezes", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Oliveira", Nada a apontar, ""),SE(Avaliacao!A1="Paula Ferreira", Nada a apontar, ""),SE(Avaliacao!A1="Paulo Vieira", Nada a apontar, ""),SE(Avaliacao!A1="Rafaela Carvalho", Nada a apontar, ""),SE(Avaliacao!A1="Catarina Milheiro", Nada a apontar, ""),SE(Avaliacao!A1="Goncalo Figueiredo", Nada a apontar, ""),SE(Avaliacao!A1="Ines Cabral", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Arezes", Nada a apontar, ""),SE(Avaliacao!A1="Mariana Oliveira", Nada a apontar, ""),SE(Avaliacao!A1="Paula Ferreira", Nada a apontar, ""),SE(Avaliacao!A1="Paulo Vieira", Nada a apontar, ""),SE(Avaliacao!A1="Rafaela Carvalho", Nada a apontar, ""),)</f>
+        <f>CONCATENAR(SE(Avaliacao!A1="Catarina Milheiro", 0.0, ""),SE(Avaliacao!A1="Goncalo Figueiredo", 0.0, ""),SE(Avaliacao!A1="Ines Cabral", 0.0, ""),SE(Avaliacao!A1="Mariana Arezes", 0.0, ""),SE(Avaliacao!A1="Mariana Oliveira", 0.0, ""),SE(Avaliacao!A1="Paula Ferreira", 0.0, ""),SE(Avaliacao!A1="Paulo Vieira", 0.0, ""),SE(Avaliacao!A1="Rafaela Carvalho", 0.0, ""),SE(Avaliacao!A1="Pedro Machado", 0.0, ""),SE(Avaliacao!A1="Beatriz Simoes", 0.0, ""),SE(Avaliacao!A1="Beatriz Sousa", 0.0, ""),SE(Avaliacao!A1="Catarina Oliveira", 0.0, ""),SE(Avaliacao!A1="Claudia Santos", 0.0, ""),SE(Avaliacao!A1="Ines Faria", 0.0, ""),SE(Avaliacao!A1="Ines Geraldes", 0.0, ""),SE(Avaliacao!A1="Leticia Santos", 0.0, ""),SE(Avaliacao!A1="Marcia Costa", 0.0, ""),SE(Avaliacao!A1="Margarida Ribeiro", 0.0, ""),SE(Avaliacao!A1="Mariana Coelho", 0.0, ""),SE(Avaliacao!A1="Raquel Baptista", 0.0, ""),)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionei logs no frontend
</commit_message>
<xml_diff>
--- a/output/result.xlsx
+++ b/output/result.xlsx
@@ -8868,9 +8868,12 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="17">
+  <dataValidations count="18">
     <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>=$B$1:$B$9</formula1>
+    </dataValidation>
+    <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=$B$1:$B$0</formula1>
     </dataValidation>
     <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>=$B$1:$B$0</formula1>

</xml_diff>

<commit_message>
ele funfa, aleluiagit add .
</commit_message>
<xml_diff>
--- a/output/result.xlsx
+++ b/output/result.xlsx
@@ -8,10 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Avaliacao-Vice-Presidente-Externo" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Avaliacao-Membro-RH" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="resultado" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Avaliacao" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Avaliacao RH" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -36,7 +33,7 @@
       <color rgb="00000000"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -63,18 +60,8 @@
         <fgColor rgb="00DDDDDD"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00cccccc"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ffffff"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="17">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -124,152 +111,11 @@
         <color rgb="00CCCCCC"/>
       </bottom>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="00CCCCCC"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="00CCCCCC"/>
-      </right>
-      <top style="thin">
-        <color rgb="00CCCCCC"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="00CCCCCC"/>
-      </right>
-      <top style="thin">
-        <color rgb="00CCCCCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="00CCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="00000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="00000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="00000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="00000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00CCCCCC"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="00CCCCCC"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00CCCCCC"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="00CCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="00CCCCCC"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="00CCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00CCCCCC"/>
-      </left>
-      <right style="thin">
-        <color rgb="00CCCCCC"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00CCCCCC"/>
-      </left>
-      <right style="thin">
-        <color rgb="00CCCCCC"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="00CCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -286,22 +132,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -685,904 +515,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Avaliação de desempenho</t>
-        </is>
-      </c>
-      <c r="B1" s="8" t="n"/>
-      <c r="C1" s="8" t="n"/>
-      <c r="D1" s="8" t="n"/>
-      <c r="E1" s="8" t="n"/>
-      <c r="F1" s="8" t="n"/>
-      <c r="G1" s="8" t="n"/>
-      <c r="H1" s="8" t="n"/>
-      <c r="I1" s="8" t="n"/>
-      <c r="J1" s="8" t="n"/>
-      <c r="K1" s="8" t="n"/>
-      <c r="L1" s="8" t="n"/>
-      <c r="M1" s="8" t="n"/>
-      <c r="N1" s="8" t="n"/>
-      <c r="O1" s="8" t="n"/>
-      <c r="P1" s="8" t="n"/>
-      <c r="Q1" s="8" t="n"/>
-      <c r="R1" s="8" t="n"/>
-      <c r="S1" s="8" t="n"/>
-      <c r="T1" s="8" t="n"/>
-      <c r="U1" s="8" t="n"/>
-      <c r="V1" s="8" t="n"/>
-      <c r="W1" s="8" t="n"/>
-      <c r="X1" s="8" t="n"/>
-      <c r="Y1" s="8" t="n"/>
-      <c r="Z1" s="8" t="n"/>
-      <c r="AA1" s="8" t="n"/>
-      <c r="AB1" s="9" t="n"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>Avaliador</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>Avaliado</t>
-        </is>
-      </c>
-      <c r="E2" s="5" t="inlineStr">
-        <is>
-          <t>O VPE coopera com os seus colegas para alcançar objetivos comuns que tenham sido estabelecidos.</t>
-        </is>
-      </c>
-      <c r="F2" s="6" t="inlineStr">
-        <is>
-          <t>O VPE assume, em regra, objetivos ambiciosos e exigentes, embora realistas, para si e para os seus colegas.</t>
-        </is>
-      </c>
-      <c r="G2" s="5" t="inlineStr">
-        <is>
-          <t>O VPE compromete-se com os resultados a alcançar de acordo com os objetivos estratégicos da júnior empresa, e é persistente perante obstáculos e dificuldades.</t>
-        </is>
-      </c>
-      <c r="H2" s="6" t="inlineStr">
-        <is>
-          <t>O VPE aceita correr riscos para atingir os resultados desejados e assume as responsabilidades pelo sucesso ou fracasso dos mesmos.</t>
-        </is>
-      </c>
-      <c r="I2" s="5" t="inlineStr">
-        <is>
-          <t>O VPE tem noção do que é prioritário para uma tarefa, respondendo, em regra, prontamente nos momentos de pressão e urgência.</t>
-        </is>
-      </c>
-      <c r="J2" s="6" t="inlineStr">
-        <is>
-          <t>O VPE procura desenvolver o seu conhecimento técnico nas áreas relevantes para o seu departamento ou projeto em que esteja envolvido, promovendo um autodesenvolvimento contínuo.</t>
-        </is>
-      </c>
-      <c r="K2" s="5" t="inlineStr">
-        <is>
-          <t>O VPE tem em conta as necessidades, requisitos e opiniões do cliente no desenvolvimento de um projeto.</t>
-        </is>
-      </c>
-      <c r="L2" s="6" t="inlineStr">
-        <is>
-          <t>O VPE sabe delegar tarefas de forma produtiva, justa e homogénea. Consegue manter uma dinâmica de departamento saudável e tem como objetivo o trabalho em equipa.</t>
-        </is>
-      </c>
-      <c r="M2" s="5" t="inlineStr">
-        <is>
-          <t>O VPE tenta obter o resultado mais vantajoso possível para os projetos e para a EPIC Júnior sem comprometer padrões éticos, senso comum e a confiança do cliente.</t>
-        </is>
-      </c>
-      <c r="N2" s="6" t="inlineStr">
-        <is>
-          <t>O VPE sabe aproveitar ao máximo e integrar os recursos disponíveis dentro da EPIC Júnior, de forma global. Consegue reavaliar, aprimorar e padronizar os processos de trabalho.</t>
-        </is>
-      </c>
-      <c r="O2" s="5" t="inlineStr">
-        <is>
-          <t>O VPE tem a capacidade de estabelecer uma rede de contactos ou uma conexão a empresas que possam ser futuros clientes.</t>
-        </is>
-      </c>
-      <c r="P2" s="6" t="inlineStr">
-        <is>
-          <t>O VPE tem a capacidade de convencer pessoas, ou mudar a sua perspetiva, usando o seu poder de argumentação, raciocínio e lógica.</t>
-        </is>
-      </c>
-      <c r="Q2" s="5" t="inlineStr">
-        <is>
-          <t>O VPE consegue estruturar o seu pensamento de forma coerente, levando a boas conclusões. Sabe desenvolver estratégias ou ideias bem planeadas/estruturadas</t>
-        </is>
-      </c>
-      <c r="R2" s="6" t="inlineStr">
-        <is>
-          <t>O VPE consegue organizar o que faz de forma eficiente e clara, exibindo uma boa gestão de tarefas e tempo.</t>
-        </is>
-      </c>
-      <c r="S2" s="5" t="inlineStr">
-        <is>
-          <t>O VPE participa regularmente em formações internas e noutras atividades recreativas promovidas pelo departamento de Recursos Humanos.</t>
-        </is>
-      </c>
-      <c r="T2" s="6" t="inlineStr">
-        <is>
-          <t>O VPE participa regularmente em reuniões gerais e reuniões de departamento.</t>
-        </is>
-      </c>
-      <c r="U2" s="5" t="inlineStr">
-        <is>
-          <t>O VPE sabe comportar-se de uma forma correta e adequada e de uma maneira profissional e respeitosa, em situações em que representa a EPIC Júnior.</t>
-        </is>
-      </c>
-      <c r="V2" s="6" t="inlineStr">
-        <is>
-          <t>O VPE respeita os valores, os membros, as instalações e todos os recursos da EPIC Júnior.</t>
-        </is>
-      </c>
-      <c r="W2" s="5" t="inlineStr">
-        <is>
-          <t>O VPE cumpre os objetivos das tarefas pelos quais é responsável.</t>
-        </is>
-      </c>
-      <c r="X2" s="6" t="inlineStr">
-        <is>
-          <t>O VPE respeita o prazo de entrega das suas tarefas.</t>
-        </is>
-      </c>
-      <c r="Y2" s="5" t="inlineStr">
-        <is>
-          <t>O VPE, caso necessário, desenvolve conhecimento técnico especifico para completar a sua tarefa.</t>
-        </is>
-      </c>
-      <c r="Z2" s="6" t="inlineStr">
-        <is>
-          <t>Em tarefas de grupo, o VPE é capaz de comunicar com os seus membros de forma clara e concisa, conseguindo defender a sua opinião mas respeitando a opinião dos outros, mantendo uma boa relação interpessoal.</t>
-        </is>
-      </c>
-      <c r="AA2" s="5" t="inlineStr">
-        <is>
-          <t>O VPE é capaz de executar a sua tarefa de forma eficaz e com qualidade, apresentando espírito crítico, ou seja, questionando e analisando-a de forma racional.</t>
-        </is>
-      </c>
-      <c r="AB2" s="6" t="inlineStr">
-        <is>
-          <t>Observações</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="inlineStr">
-        <is>
-          <t>Liliana Freitas</t>
-        </is>
-      </c>
-      <c r="B3" s="10" t="n"/>
-      <c r="C3" s="5" t="inlineStr">
-        <is>
-          <t>Pedro Machado</t>
-        </is>
-      </c>
-      <c r="D3" s="10" t="n"/>
-      <c r="E3" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F3" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="G3" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="H3" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="I3" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="J3" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="K3" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="L3" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="M3" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="N3" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="O3" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="P3" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q3" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="R3" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="S3" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="T3" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="U3" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="V3" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="W3" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="X3" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="Y3" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="Z3" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="AA3" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="AB3" s="6" t="inlineStr">
-        <is>
-          <t>Nada a apontar</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="5" t="inlineStr">
-        <is>
-          <t>Francisco Sousa</t>
-        </is>
-      </c>
-      <c r="B4" s="10" t="n"/>
-      <c r="C4" s="5" t="inlineStr">
-        <is>
-          <t>Pedro Machado</t>
-        </is>
-      </c>
-      <c r="D4" s="10" t="n"/>
-      <c r="E4" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F4" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="G4" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="H4" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="I4" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="J4" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="K4" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="L4" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="M4" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="N4" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="O4" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="P4" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q4" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="R4" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="S4" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="T4" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="U4" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="V4" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="W4" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="X4" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="Y4" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="Z4" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="AA4" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="AB4" s="6" t="inlineStr">
-        <is>
-          <t>Nada a apontar</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="inlineStr">
-        <is>
-          <t>Joana Alves</t>
-        </is>
-      </c>
-      <c r="B5" s="10" t="n"/>
-      <c r="C5" s="5" t="inlineStr">
-        <is>
-          <t>Pedro Machado</t>
-        </is>
-      </c>
-      <c r="D5" s="10" t="n"/>
-      <c r="E5" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F5" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="H5" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="I5" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="J5" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="K5" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="L5" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="M5" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="N5" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="O5" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="P5" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q5" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="R5" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="S5" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="T5" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="U5" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="V5" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="W5" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="X5" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="Y5" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="Z5" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="AA5" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="AB5" s="6" t="inlineStr">
-        <is>
-          <t>Nada a apontar</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="5" t="inlineStr">
-        <is>
-          <t>Pedro Machado</t>
-        </is>
-      </c>
-      <c r="B6" s="10" t="n"/>
-      <c r="C6" s="5" t="inlineStr">
-        <is>
-          <t>Pedro Machado</t>
-        </is>
-      </c>
-      <c r="D6" s="10" t="n"/>
-      <c r="E6" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F6" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="G6" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="H6" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="I6" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="J6" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="K6" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="L6" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="M6" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="N6" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="O6" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="P6" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q6" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="R6" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="S6" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="T6" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="U6" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="V6" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="W6" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="X6" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="Y6" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="Z6" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="AA6" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="AB6" s="6" t="inlineStr">
-        <is>
-          <t>(espero continuar a demonstrar resultados, a melhorar sempre em prol da EPIC Júnior)</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="5" t="inlineStr">
-        <is>
-          <t>Catarina Oliveira</t>
-        </is>
-      </c>
-      <c r="B7" s="10" t="n"/>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>Pedro Machado</t>
-        </is>
-      </c>
-      <c r="D7" s="10" t="n"/>
-      <c r="E7" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F7" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="G7" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="H7" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="I7" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="J7" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="K7" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="L7" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="M7" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="N7" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="O7" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="P7" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q7" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="R7" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="S7" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="T7" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="U7" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="V7" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="W7" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="X7" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="Y7" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="Z7" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="AA7" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="AB7" s="6" t="inlineStr">
-        <is>
-          <t>Nada a apontar</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="5" t="inlineStr">
-        <is>
-          <t>Filipe Araújo</t>
-        </is>
-      </c>
-      <c r="B8" s="10" t="n"/>
-      <c r="C8" s="5" t="inlineStr">
-        <is>
-          <t>Pedro Machado</t>
-        </is>
-      </c>
-      <c r="D8" s="10" t="n"/>
-      <c r="E8" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F8" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="G8" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="H8" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="I8" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="J8" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="K8" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="L8" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="M8" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="N8" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="O8" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="P8" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q8" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="R8" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="S8" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="T8" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="U8" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="V8" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="W8" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="X8" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="Y8" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="Z8" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="AA8" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="AB8" s="6" t="inlineStr">
-        <is>
-          <t>De facto, estou muito satisfeito com o trabalho do Pedro e a minha avaliação transparece esse mesmo reconhecimento. Na questão "O VPE participa regularmente em reuniões gerais e reuniões de departamento.” assumi que fossem reuniões de direção.</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="183">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="I8"/>
-    <mergeCell ref="P3"/>
-    <mergeCell ref="H3"/>
-    <mergeCell ref="J3"/>
-    <mergeCell ref="E7"/>
-    <mergeCell ref="T6"/>
-    <mergeCell ref="W2"/>
-    <mergeCell ref="P5"/>
-    <mergeCell ref="H5"/>
-    <mergeCell ref="R5"/>
-    <mergeCell ref="Y8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AA8"/>
-    <mergeCell ref="N4"/>
-    <mergeCell ref="Z6"/>
-    <mergeCell ref="P4"/>
-    <mergeCell ref="AB6"/>
-    <mergeCell ref="G2"/>
-    <mergeCell ref="I2"/>
-    <mergeCell ref="H4"/>
-    <mergeCell ref="R4"/>
-    <mergeCell ref="T4"/>
-    <mergeCell ref="S3"/>
-    <mergeCell ref="V4"/>
-    <mergeCell ref="H6"/>
-    <mergeCell ref="X7"/>
-    <mergeCell ref="J6"/>
-    <mergeCell ref="M2"/>
-    <mergeCell ref="Z7"/>
-    <mergeCell ref="A1:AB1"/>
-    <mergeCell ref="P8"/>
-    <mergeCell ref="O5"/>
-    <mergeCell ref="Y5"/>
-    <mergeCell ref="Y2"/>
-    <mergeCell ref="Q5"/>
-    <mergeCell ref="G6"/>
-    <mergeCell ref="L8"/>
-    <mergeCell ref="N8"/>
-    <mergeCell ref="U3"/>
-    <mergeCell ref="M6"/>
-    <mergeCell ref="E6"/>
-    <mergeCell ref="H7"/>
-    <mergeCell ref="J7"/>
-    <mergeCell ref="K8"/>
-    <mergeCell ref="Y6"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="R3"/>
-    <mergeCell ref="T8"/>
-    <mergeCell ref="G4"/>
-    <mergeCell ref="AA3"/>
-    <mergeCell ref="I4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="K7"/>
-    <mergeCell ref="R2"/>
-    <mergeCell ref="J2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="K4"/>
-    <mergeCell ref="M4"/>
-    <mergeCell ref="AB3"/>
-    <mergeCell ref="T3"/>
-    <mergeCell ref="W4"/>
-    <mergeCell ref="O7"/>
-    <mergeCell ref="V3"/>
-    <mergeCell ref="Y4"/>
-    <mergeCell ref="Q7"/>
-    <mergeCell ref="O6"/>
-    <mergeCell ref="J5"/>
-    <mergeCell ref="AB5"/>
-    <mergeCell ref="T5"/>
-    <mergeCell ref="V5"/>
-    <mergeCell ref="E8"/>
-    <mergeCell ref="G8"/>
-    <mergeCell ref="AB4"/>
-    <mergeCell ref="N3"/>
-    <mergeCell ref="Q8"/>
-    <mergeCell ref="F3"/>
-    <mergeCell ref="S8"/>
-    <mergeCell ref="P6"/>
-    <mergeCell ref="S2"/>
-    <mergeCell ref="R6"/>
-    <mergeCell ref="U2"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="L5"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="N5"/>
-    <mergeCell ref="W3"/>
-    <mergeCell ref="G3"/>
-    <mergeCell ref="J4"/>
-    <mergeCell ref="V6"/>
-    <mergeCell ref="I3"/>
-    <mergeCell ref="L4"/>
-    <mergeCell ref="X6"/>
-    <mergeCell ref="P7"/>
-    <mergeCell ref="E2"/>
-    <mergeCell ref="G5"/>
-    <mergeCell ref="I5"/>
-    <mergeCell ref="M3"/>
-    <mergeCell ref="AB8"/>
-    <mergeCell ref="T7"/>
-    <mergeCell ref="V7"/>
-    <mergeCell ref="AA2"/>
-    <mergeCell ref="S5"/>
-    <mergeCell ref="U5"/>
-    <mergeCell ref="S4"/>
-    <mergeCell ref="H8"/>
-    <mergeCell ref="U4"/>
-    <mergeCell ref="J8"/>
-    <mergeCell ref="O3"/>
-    <mergeCell ref="Q3"/>
-    <mergeCell ref="L2"/>
-    <mergeCell ref="I6"/>
-    <mergeCell ref="V2"/>
-    <mergeCell ref="U6"/>
-    <mergeCell ref="X2"/>
-    <mergeCell ref="W6"/>
-    <mergeCell ref="F6"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="E4"/>
-    <mergeCell ref="L3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="AA6"/>
-    <mergeCell ref="G7"/>
-    <mergeCell ref="I7"/>
-    <mergeCell ref="P2"/>
-    <mergeCell ref="S7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="X3"/>
-    <mergeCell ref="Z3"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="M7"/>
-    <mergeCell ref="Y7"/>
-    <mergeCell ref="AA7"/>
-    <mergeCell ref="X5"/>
-    <mergeCell ref="K2"/>
-    <mergeCell ref="Z5"/>
-    <mergeCell ref="U8"/>
-    <mergeCell ref="X4"/>
-    <mergeCell ref="M8"/>
-    <mergeCell ref="Z4"/>
-    <mergeCell ref="W8"/>
-    <mergeCell ref="O8"/>
-    <mergeCell ref="L6"/>
-    <mergeCell ref="O2"/>
-    <mergeCell ref="AB7"/>
-    <mergeCell ref="N6"/>
-    <mergeCell ref="Q2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K6"/>
-    <mergeCell ref="K3"/>
-    <mergeCell ref="F4"/>
-    <mergeCell ref="E3"/>
-    <mergeCell ref="R8"/>
-    <mergeCell ref="Y3"/>
-    <mergeCell ref="L7"/>
-    <mergeCell ref="N7"/>
-    <mergeCell ref="K5"/>
-    <mergeCell ref="M5"/>
-    <mergeCell ref="E5"/>
-    <mergeCell ref="W5"/>
-    <mergeCell ref="V8"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F7"/>
-    <mergeCell ref="X8"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="R7"/>
-    <mergeCell ref="AA5"/>
-    <mergeCell ref="N2"/>
-    <mergeCell ref="F5"/>
-    <mergeCell ref="O4"/>
-    <mergeCell ref="Q4"/>
-    <mergeCell ref="F8"/>
-    <mergeCell ref="F2"/>
-    <mergeCell ref="AA4"/>
-    <mergeCell ref="H2"/>
-    <mergeCell ref="U7"/>
-    <mergeCell ref="Z8"/>
-    <mergeCell ref="Z2"/>
-    <mergeCell ref="W7"/>
-    <mergeCell ref="AB2"/>
-    <mergeCell ref="Q6"/>
-    <mergeCell ref="T2"/>
-    <mergeCell ref="S6"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:X74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1597,29 +529,29 @@
           <t>Avaliação de desempenho</t>
         </is>
       </c>
-      <c r="B1" s="8" t="n"/>
-      <c r="C1" s="8" t="n"/>
-      <c r="D1" s="8" t="n"/>
-      <c r="E1" s="8" t="n"/>
-      <c r="F1" s="8" t="n"/>
-      <c r="G1" s="8" t="n"/>
-      <c r="H1" s="8" t="n"/>
-      <c r="I1" s="8" t="n"/>
-      <c r="J1" s="8" t="n"/>
-      <c r="K1" s="8" t="n"/>
-      <c r="L1" s="8" t="n"/>
-      <c r="M1" s="8" t="n"/>
-      <c r="N1" s="8" t="n"/>
-      <c r="O1" s="8" t="n"/>
-      <c r="P1" s="8" t="n"/>
-      <c r="Q1" s="8" t="n"/>
-      <c r="R1" s="8" t="n"/>
-      <c r="S1" s="8" t="n"/>
-      <c r="T1" s="8" t="n"/>
-      <c r="U1" s="8" t="n"/>
-      <c r="V1" s="8" t="n"/>
-      <c r="W1" s="8" t="n"/>
-      <c r="X1" s="9" t="n"/>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="2" t="n"/>
+      <c r="P1" s="2" t="n"/>
+      <c r="Q1" s="2" t="n"/>
+      <c r="R1" s="2" t="n"/>
+      <c r="S1" s="2" t="n"/>
+      <c r="T1" s="2" t="n"/>
+      <c r="U1" s="2" t="n"/>
+      <c r="V1" s="2" t="n"/>
+      <c r="W1" s="2" t="n"/>
+      <c r="X1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -1627,11 +559,13 @@
           <t>Avaliador</t>
         </is>
       </c>
+      <c r="B2" s="4" t="n"/>
       <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Avaliado</t>
         </is>
       </c>
+      <c r="D2" s="4" t="n"/>
       <c r="E2" s="5" t="inlineStr">
         <is>
           <t>1. O membro coopera com os seus colegas para alcançar objetivos comuns que tenham sido estabelecidos.</t>
@@ -1739,13 +673,13 @@
           <t>Rafaela Carvalho</t>
         </is>
       </c>
-      <c r="B3" s="11" t="n"/>
+      <c r="B3" s="7" t="n"/>
       <c r="C3" s="5" t="inlineStr">
         <is>
           <t>Catarina Milheiro</t>
         </is>
       </c>
-      <c r="D3" s="10" t="n"/>
+      <c r="D3" s="7" t="n"/>
       <c r="E3" s="5" t="n">
         <v>6</v>
       </c>
@@ -1810,14 +744,13 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="12" t="n"/>
-      <c r="B4" s="13" t="n"/>
+      <c r="A4" s="7" t="n"/>
       <c r="C4" s="5" t="inlineStr">
         <is>
           <t>Goncalo Figueiredo</t>
         </is>
       </c>
-      <c r="D4" s="10" t="n"/>
+      <c r="D4" s="7" t="n"/>
       <c r="E4" s="5" t="n">
         <v>5</v>
       </c>
@@ -1875,17 +808,16 @@
       <c r="W4" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="X4" s="14" t="n"/>
+      <c r="X4" s="7" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="12" t="n"/>
-      <c r="B5" s="13" t="n"/>
+      <c r="A5" s="7" t="n"/>
       <c r="C5" s="5" t="inlineStr">
         <is>
           <t>Ines Cabral</t>
         </is>
       </c>
-      <c r="D5" s="10" t="n"/>
+      <c r="D5" s="7" t="n"/>
       <c r="E5" s="5" t="n">
         <v>5</v>
       </c>
@@ -1943,17 +875,16 @@
       <c r="W5" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="X5" s="14" t="n"/>
+      <c r="X5" s="7" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="n"/>
-      <c r="B6" s="13" t="n"/>
+      <c r="A6" s="7" t="n"/>
       <c r="C6" s="5" t="inlineStr">
         <is>
           <t>Mariana Arezes</t>
         </is>
       </c>
-      <c r="D6" s="10" t="n"/>
+      <c r="D6" s="7" t="n"/>
       <c r="E6" s="5" t="n">
         <v>6</v>
       </c>
@@ -2011,17 +942,16 @@
       <c r="W6" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="X6" s="14" t="n"/>
+      <c r="X6" s="7" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="n"/>
-      <c r="B7" s="13" t="n"/>
+      <c r="A7" s="7" t="n"/>
       <c r="C7" s="5" t="inlineStr">
         <is>
           <t>Mariana Oliveira</t>
         </is>
       </c>
-      <c r="D7" s="10" t="n"/>
+      <c r="D7" s="7" t="n"/>
       <c r="E7" s="5" t="n">
         <v>6</v>
       </c>
@@ -2079,17 +1009,16 @@
       <c r="W7" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X7" s="14" t="n"/>
+      <c r="X7" s="7" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="12" t="n"/>
-      <c r="B8" s="13" t="n"/>
+      <c r="A8" s="7" t="n"/>
       <c r="C8" s="5" t="inlineStr">
         <is>
           <t>Paula Ferreira</t>
         </is>
       </c>
-      <c r="D8" s="10" t="n"/>
+      <c r="D8" s="7" t="n"/>
       <c r="E8" s="5" t="n">
         <v>6</v>
       </c>
@@ -2147,17 +1076,16 @@
       <c r="W8" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X8" s="14" t="n"/>
+      <c r="X8" s="7" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="12" t="n"/>
-      <c r="B9" s="13" t="n"/>
+      <c r="A9" s="7" t="n"/>
       <c r="C9" s="5" t="inlineStr">
         <is>
           <t>Paulo Vieira</t>
         </is>
       </c>
-      <c r="D9" s="10" t="n"/>
+      <c r="D9" s="7" t="n"/>
       <c r="E9" s="5" t="n">
         <v>5</v>
       </c>
@@ -2215,17 +1143,16 @@
       <c r="W9" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="X9" s="14" t="n"/>
+      <c r="X9" s="7" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="15" t="n"/>
-      <c r="B10" s="16" t="n"/>
+      <c r="A10" s="7" t="n"/>
       <c r="C10" s="5" t="inlineStr">
         <is>
           <t>Rafaela Carvalho</t>
         </is>
       </c>
-      <c r="D10" s="10" t="n"/>
+      <c r="D10" s="7" t="n"/>
       <c r="E10" s="5" t="n">
         <v>5</v>
       </c>
@@ -2283,7 +1210,7 @@
       <c r="W10" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="X10" s="17" t="n"/>
+      <c r="X10" s="7" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="inlineStr">
@@ -2291,13 +1218,13 @@
           <t>Paula Ferreira</t>
         </is>
       </c>
-      <c r="B11" s="11" t="n"/>
+      <c r="B11" s="7" t="n"/>
       <c r="C11" s="5" t="inlineStr">
         <is>
           <t>Catarina Milheiro</t>
         </is>
       </c>
-      <c r="D11" s="10" t="n"/>
+      <c r="D11" s="7" t="n"/>
       <c r="E11" s="5" t="n">
         <v>6</v>
       </c>
@@ -2362,14 +1289,13 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="12" t="n"/>
-      <c r="B12" s="13" t="n"/>
+      <c r="A12" s="7" t="n"/>
       <c r="C12" s="5" t="inlineStr">
         <is>
           <t>Goncalo Figueiredo</t>
         </is>
       </c>
-      <c r="D12" s="10" t="n"/>
+      <c r="D12" s="7" t="n"/>
       <c r="E12" s="5" t="n">
         <v>4</v>
       </c>
@@ -2427,17 +1353,16 @@
       <c r="W12" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="X12" s="14" t="n"/>
+      <c r="X12" s="7" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="12" t="n"/>
-      <c r="B13" s="13" t="n"/>
+      <c r="A13" s="7" t="n"/>
       <c r="C13" s="5" t="inlineStr">
         <is>
           <t>Ines Cabral</t>
         </is>
       </c>
-      <c r="D13" s="10" t="n"/>
+      <c r="D13" s="7" t="n"/>
       <c r="E13" s="5" t="n">
         <v>4</v>
       </c>
@@ -2495,17 +1420,16 @@
       <c r="W13" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="X13" s="14" t="n"/>
+      <c r="X13" s="7" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="12" t="n"/>
-      <c r="B14" s="13" t="n"/>
+      <c r="A14" s="7" t="n"/>
       <c r="C14" s="5" t="inlineStr">
         <is>
           <t>Mariana Arezes</t>
         </is>
       </c>
-      <c r="D14" s="10" t="n"/>
+      <c r="D14" s="7" t="n"/>
       <c r="E14" s="5" t="n">
         <v>5</v>
       </c>
@@ -2563,17 +1487,16 @@
       <c r="W14" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X14" s="14" t="n"/>
+      <c r="X14" s="7" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="12" t="n"/>
-      <c r="B15" s="13" t="n"/>
+      <c r="A15" s="7" t="n"/>
       <c r="C15" s="5" t="inlineStr">
         <is>
           <t>Mariana Oliveira</t>
         </is>
       </c>
-      <c r="D15" s="10" t="n"/>
+      <c r="D15" s="7" t="n"/>
       <c r="E15" s="5" t="n">
         <v>6</v>
       </c>
@@ -2631,17 +1554,16 @@
       <c r="W15" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X15" s="14" t="n"/>
+      <c r="X15" s="7" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="12" t="n"/>
-      <c r="B16" s="13" t="n"/>
+      <c r="A16" s="7" t="n"/>
       <c r="C16" s="5" t="inlineStr">
         <is>
           <t>Paula Ferreira</t>
         </is>
       </c>
-      <c r="D16" s="10" t="n"/>
+      <c r="D16" s="7" t="n"/>
       <c r="E16" s="5" t="n">
         <v>6</v>
       </c>
@@ -2699,17 +1621,16 @@
       <c r="W16" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X16" s="14" t="n"/>
+      <c r="X16" s="7" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="12" t="n"/>
-      <c r="B17" s="13" t="n"/>
+      <c r="A17" s="7" t="n"/>
       <c r="C17" s="5" t="inlineStr">
         <is>
           <t>Paulo Vieira</t>
         </is>
       </c>
-      <c r="D17" s="10" t="n"/>
+      <c r="D17" s="7" t="n"/>
       <c r="E17" s="5" t="n">
         <v>5</v>
       </c>
@@ -2767,17 +1688,16 @@
       <c r="W17" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="X17" s="14" t="n"/>
+      <c r="X17" s="7" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="15" t="n"/>
-      <c r="B18" s="16" t="n"/>
+      <c r="A18" s="7" t="n"/>
       <c r="C18" s="5" t="inlineStr">
         <is>
           <t>Rafaela Carvalho</t>
         </is>
       </c>
-      <c r="D18" s="10" t="n"/>
+      <c r="D18" s="7" t="n"/>
       <c r="E18" s="5" t="n">
         <v>6</v>
       </c>
@@ -2835,7 +1755,7 @@
       <c r="W18" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="X18" s="17" t="n"/>
+      <c r="X18" s="7" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="inlineStr">
@@ -2843,13 +1763,13 @@
           <t>Mariana Oliveira</t>
         </is>
       </c>
-      <c r="B19" s="11" t="n"/>
+      <c r="B19" s="7" t="n"/>
       <c r="C19" s="5" t="inlineStr">
         <is>
           <t>Catarina Milheiro</t>
         </is>
       </c>
-      <c r="D19" s="10" t="n"/>
+      <c r="D19" s="7" t="n"/>
       <c r="E19" s="5" t="n">
         <v>6</v>
       </c>
@@ -2914,14 +1834,13 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="12" t="n"/>
-      <c r="B20" s="13" t="n"/>
+      <c r="A20" s="7" t="n"/>
       <c r="C20" s="5" t="inlineStr">
         <is>
           <t>Goncalo Figueiredo</t>
         </is>
       </c>
-      <c r="D20" s="10" t="n"/>
+      <c r="D20" s="7" t="n"/>
       <c r="E20" s="5" t="n">
         <v>3</v>
       </c>
@@ -2979,17 +1898,16 @@
       <c r="W20" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="X20" s="14" t="n"/>
+      <c r="X20" s="7" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="12" t="n"/>
-      <c r="B21" s="13" t="n"/>
+      <c r="A21" s="7" t="n"/>
       <c r="C21" s="5" t="inlineStr">
         <is>
           <t>Ines Cabral</t>
         </is>
       </c>
-      <c r="D21" s="10" t="n"/>
+      <c r="D21" s="7" t="n"/>
       <c r="E21" s="5" t="n">
         <v>5</v>
       </c>
@@ -3047,17 +1965,16 @@
       <c r="W21" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="X21" s="14" t="n"/>
+      <c r="X21" s="7" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="12" t="n"/>
-      <c r="B22" s="13" t="n"/>
+      <c r="A22" s="7" t="n"/>
       <c r="C22" s="5" t="inlineStr">
         <is>
           <t>Mariana Arezes</t>
         </is>
       </c>
-      <c r="D22" s="10" t="n"/>
+      <c r="D22" s="7" t="n"/>
       <c r="E22" s="5" t="n">
         <v>6</v>
       </c>
@@ -3115,17 +2032,16 @@
       <c r="W22" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X22" s="14" t="n"/>
+      <c r="X22" s="7" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="12" t="n"/>
-      <c r="B23" s="13" t="n"/>
+      <c r="A23" s="7" t="n"/>
       <c r="C23" s="5" t="inlineStr">
         <is>
           <t>Mariana Oliveira</t>
         </is>
       </c>
-      <c r="D23" s="10" t="n"/>
+      <c r="D23" s="7" t="n"/>
       <c r="E23" s="5" t="n">
         <v>6</v>
       </c>
@@ -3183,17 +2099,16 @@
       <c r="W23" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X23" s="14" t="n"/>
+      <c r="X23" s="7" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="12" t="n"/>
-      <c r="B24" s="13" t="n"/>
+      <c r="A24" s="7" t="n"/>
       <c r="C24" s="5" t="inlineStr">
         <is>
           <t>Paula Ferreira</t>
         </is>
       </c>
-      <c r="D24" s="10" t="n"/>
+      <c r="D24" s="7" t="n"/>
       <c r="E24" s="5" t="n">
         <v>6</v>
       </c>
@@ -3251,17 +2166,16 @@
       <c r="W24" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X24" s="14" t="n"/>
+      <c r="X24" s="7" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="12" t="n"/>
-      <c r="B25" s="13" t="n"/>
+      <c r="A25" s="7" t="n"/>
       <c r="C25" s="5" t="inlineStr">
         <is>
           <t>Paulo Vieira</t>
         </is>
       </c>
-      <c r="D25" s="10" t="n"/>
+      <c r="D25" s="7" t="n"/>
       <c r="E25" s="5" t="n">
         <v>6</v>
       </c>
@@ -3319,17 +2233,16 @@
       <c r="W25" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X25" s="14" t="n"/>
+      <c r="X25" s="7" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="15" t="n"/>
-      <c r="B26" s="16" t="n"/>
+      <c r="A26" s="7" t="n"/>
       <c r="C26" s="5" t="inlineStr">
         <is>
           <t>Rafaela Carvalho</t>
         </is>
       </c>
-      <c r="D26" s="10" t="n"/>
+      <c r="D26" s="7" t="n"/>
       <c r="E26" s="5" t="n">
         <v>5</v>
       </c>
@@ -3387,7 +2300,7 @@
       <c r="W26" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="X26" s="17" t="n"/>
+      <c r="X26" s="7" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="5" t="inlineStr">
@@ -3395,13 +2308,13 @@
           <t>Inês Cabral</t>
         </is>
       </c>
-      <c r="B27" s="11" t="n"/>
+      <c r="B27" s="7" t="n"/>
       <c r="C27" s="5" t="inlineStr">
         <is>
           <t>Catarina Milheiro</t>
         </is>
       </c>
-      <c r="D27" s="10" t="n"/>
+      <c r="D27" s="7" t="n"/>
       <c r="E27" s="5" t="n">
         <v>6</v>
       </c>
@@ -3466,14 +2379,13 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="12" t="n"/>
-      <c r="B28" s="13" t="n"/>
+      <c r="A28" s="7" t="n"/>
       <c r="C28" s="5" t="inlineStr">
         <is>
           <t>Goncalo Figueiredo</t>
         </is>
       </c>
-      <c r="D28" s="10" t="n"/>
+      <c r="D28" s="7" t="n"/>
       <c r="E28" s="5" t="n">
         <v>6</v>
       </c>
@@ -3531,17 +2443,16 @@
       <c r="W28" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X28" s="14" t="n"/>
+      <c r="X28" s="7" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="12" t="n"/>
-      <c r="B29" s="13" t="n"/>
+      <c r="A29" s="7" t="n"/>
       <c r="C29" s="5" t="inlineStr">
         <is>
           <t>Ines Cabral</t>
         </is>
       </c>
-      <c r="D29" s="10" t="n"/>
+      <c r="D29" s="7" t="n"/>
       <c r="E29" s="5" t="n">
         <v>6</v>
       </c>
@@ -3599,17 +2510,16 @@
       <c r="W29" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X29" s="14" t="n"/>
+      <c r="X29" s="7" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="12" t="n"/>
-      <c r="B30" s="13" t="n"/>
+      <c r="A30" s="7" t="n"/>
       <c r="C30" s="5" t="inlineStr">
         <is>
           <t>Mariana Arezes</t>
         </is>
       </c>
-      <c r="D30" s="10" t="n"/>
+      <c r="D30" s="7" t="n"/>
       <c r="E30" s="5" t="n">
         <v>6</v>
       </c>
@@ -3667,17 +2577,16 @@
       <c r="W30" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X30" s="14" t="n"/>
+      <c r="X30" s="7" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="12" t="n"/>
-      <c r="B31" s="13" t="n"/>
+      <c r="A31" s="7" t="n"/>
       <c r="C31" s="5" t="inlineStr">
         <is>
           <t>Mariana Oliveira</t>
         </is>
       </c>
-      <c r="D31" s="10" t="n"/>
+      <c r="D31" s="7" t="n"/>
       <c r="E31" s="5" t="n">
         <v>6</v>
       </c>
@@ -3735,17 +2644,16 @@
       <c r="W31" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X31" s="14" t="n"/>
+      <c r="X31" s="7" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="12" t="n"/>
-      <c r="B32" s="13" t="n"/>
+      <c r="A32" s="7" t="n"/>
       <c r="C32" s="5" t="inlineStr">
         <is>
           <t>Paula Ferreira</t>
         </is>
       </c>
-      <c r="D32" s="10" t="n"/>
+      <c r="D32" s="7" t="n"/>
       <c r="E32" s="5" t="n">
         <v>6</v>
       </c>
@@ -3803,17 +2711,16 @@
       <c r="W32" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X32" s="14" t="n"/>
+      <c r="X32" s="7" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="12" t="n"/>
-      <c r="B33" s="13" t="n"/>
+      <c r="A33" s="7" t="n"/>
       <c r="C33" s="5" t="inlineStr">
         <is>
           <t>Paulo Vieira</t>
         </is>
       </c>
-      <c r="D33" s="10" t="n"/>
+      <c r="D33" s="7" t="n"/>
       <c r="E33" s="5" t="n">
         <v>6</v>
       </c>
@@ -3871,17 +2778,16 @@
       <c r="W33" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X33" s="14" t="n"/>
+      <c r="X33" s="7" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="15" t="n"/>
-      <c r="B34" s="16" t="n"/>
+      <c r="A34" s="7" t="n"/>
       <c r="C34" s="5" t="inlineStr">
         <is>
           <t>Rafaela Carvalho</t>
         </is>
       </c>
-      <c r="D34" s="10" t="n"/>
+      <c r="D34" s="7" t="n"/>
       <c r="E34" s="5" t="n">
         <v>6</v>
       </c>
@@ -3939,7 +2845,7 @@
       <c r="W34" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X34" s="17" t="n"/>
+      <c r="X34" s="7" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="5" t="inlineStr">
@@ -3947,13 +2853,13 @@
           <t>Mariana Arezes</t>
         </is>
       </c>
-      <c r="B35" s="11" t="n"/>
+      <c r="B35" s="7" t="n"/>
       <c r="C35" s="5" t="inlineStr">
         <is>
           <t>Catarina Milheiro</t>
         </is>
       </c>
-      <c r="D35" s="10" t="n"/>
+      <c r="D35" s="7" t="n"/>
       <c r="E35" s="5" t="n">
         <v>6</v>
       </c>
@@ -4018,14 +2924,13 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="12" t="n"/>
-      <c r="B36" s="13" t="n"/>
+      <c r="A36" s="7" t="n"/>
       <c r="C36" s="5" t="inlineStr">
         <is>
           <t>Goncalo Figueiredo</t>
         </is>
       </c>
-      <c r="D36" s="10" t="n"/>
+      <c r="D36" s="7" t="n"/>
       <c r="E36" s="5" t="n">
         <v>5</v>
       </c>
@@ -4083,17 +2988,16 @@
       <c r="W36" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="X36" s="14" t="n"/>
+      <c r="X36" s="7" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="12" t="n"/>
-      <c r="B37" s="13" t="n"/>
+      <c r="A37" s="7" t="n"/>
       <c r="C37" s="5" t="inlineStr">
         <is>
           <t>Ines Cabral</t>
         </is>
       </c>
-      <c r="D37" s="10" t="n"/>
+      <c r="D37" s="7" t="n"/>
       <c r="E37" s="5" t="n">
         <v>6</v>
       </c>
@@ -4151,17 +3055,16 @@
       <c r="W37" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="X37" s="14" t="n"/>
+      <c r="X37" s="7" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="12" t="n"/>
-      <c r="B38" s="13" t="n"/>
+      <c r="A38" s="7" t="n"/>
       <c r="C38" s="5" t="inlineStr">
         <is>
           <t>Mariana Arezes</t>
         </is>
       </c>
-      <c r="D38" s="10" t="n"/>
+      <c r="D38" s="7" t="n"/>
       <c r="E38" s="5" t="n">
         <v>5</v>
       </c>
@@ -4219,17 +3122,16 @@
       <c r="W38" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X38" s="14" t="n"/>
+      <c r="X38" s="7" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="12" t="n"/>
-      <c r="B39" s="13" t="n"/>
+      <c r="A39" s="7" t="n"/>
       <c r="C39" s="5" t="inlineStr">
         <is>
           <t>Mariana Oliveira</t>
         </is>
       </c>
-      <c r="D39" s="10" t="n"/>
+      <c r="D39" s="7" t="n"/>
       <c r="E39" s="5" t="n">
         <v>6</v>
       </c>
@@ -4287,17 +3189,16 @@
       <c r="W39" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X39" s="14" t="n"/>
+      <c r="X39" s="7" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="12" t="n"/>
-      <c r="B40" s="13" t="n"/>
+      <c r="A40" s="7" t="n"/>
       <c r="C40" s="5" t="inlineStr">
         <is>
           <t>Paula Ferreira</t>
         </is>
       </c>
-      <c r="D40" s="10" t="n"/>
+      <c r="D40" s="7" t="n"/>
       <c r="E40" s="5" t="n">
         <v>6</v>
       </c>
@@ -4355,17 +3256,16 @@
       <c r="W40" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X40" s="14" t="n"/>
+      <c r="X40" s="7" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="12" t="n"/>
-      <c r="B41" s="13" t="n"/>
+      <c r="A41" s="7" t="n"/>
       <c r="C41" s="5" t="inlineStr">
         <is>
           <t>Paulo Vieira</t>
         </is>
       </c>
-      <c r="D41" s="10" t="n"/>
+      <c r="D41" s="7" t="n"/>
       <c r="E41" s="5" t="n">
         <v>5</v>
       </c>
@@ -4423,17 +3323,16 @@
       <c r="W41" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="X41" s="14" t="n"/>
+      <c r="X41" s="7" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="15" t="n"/>
-      <c r="B42" s="16" t="n"/>
+      <c r="A42" s="7" t="n"/>
       <c r="C42" s="5" t="inlineStr">
         <is>
           <t>Rafaela Carvalho</t>
         </is>
       </c>
-      <c r="D42" s="10" t="n"/>
+      <c r="D42" s="7" t="n"/>
       <c r="E42" s="5" t="n">
         <v>5</v>
       </c>
@@ -4491,7 +3390,7 @@
       <c r="W42" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="X42" s="17" t="n"/>
+      <c r="X42" s="7" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="5" t="inlineStr">
@@ -4499,13 +3398,13 @@
           <t>Paulo Vieira</t>
         </is>
       </c>
-      <c r="B43" s="11" t="n"/>
+      <c r="B43" s="7" t="n"/>
       <c r="C43" s="5" t="inlineStr">
         <is>
           <t>Catarina Milheiro</t>
         </is>
       </c>
-      <c r="D43" s="10" t="n"/>
+      <c r="D43" s="7" t="n"/>
       <c r="E43" s="5" t="n">
         <v>6</v>
       </c>
@@ -4570,14 +3469,13 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="12" t="n"/>
-      <c r="B44" s="13" t="n"/>
+      <c r="A44" s="7" t="n"/>
       <c r="C44" s="5" t="inlineStr">
         <is>
           <t>Goncalo Figueiredo</t>
         </is>
       </c>
-      <c r="D44" s="10" t="n"/>
+      <c r="D44" s="7" t="n"/>
       <c r="E44" s="5" t="n">
         <v>5</v>
       </c>
@@ -4635,17 +3533,16 @@
       <c r="W44" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="X44" s="14" t="n"/>
+      <c r="X44" s="7" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" s="12" t="n"/>
-      <c r="B45" s="13" t="n"/>
+      <c r="A45" s="7" t="n"/>
       <c r="C45" s="5" t="inlineStr">
         <is>
           <t>Ines Cabral</t>
         </is>
       </c>
-      <c r="D45" s="10" t="n"/>
+      <c r="D45" s="7" t="n"/>
       <c r="E45" s="5" t="n">
         <v>5</v>
       </c>
@@ -4703,17 +3600,16 @@
       <c r="W45" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="X45" s="14" t="n"/>
+      <c r="X45" s="7" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="12" t="n"/>
-      <c r="B46" s="13" t="n"/>
+      <c r="A46" s="7" t="n"/>
       <c r="C46" s="5" t="inlineStr">
         <is>
           <t>Mariana Arezes</t>
         </is>
       </c>
-      <c r="D46" s="10" t="n"/>
+      <c r="D46" s="7" t="n"/>
       <c r="E46" s="5" t="n">
         <v>5</v>
       </c>
@@ -4771,17 +3667,16 @@
       <c r="W46" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="X46" s="14" t="n"/>
+      <c r="X46" s="7" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="12" t="n"/>
-      <c r="B47" s="13" t="n"/>
+      <c r="A47" s="7" t="n"/>
       <c r="C47" s="5" t="inlineStr">
         <is>
           <t>Mariana Oliveira</t>
         </is>
       </c>
-      <c r="D47" s="10" t="n"/>
+      <c r="D47" s="7" t="n"/>
       <c r="E47" s="5" t="n">
         <v>6</v>
       </c>
@@ -4839,17 +3734,16 @@
       <c r="W47" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="X47" s="14" t="n"/>
+      <c r="X47" s="7" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="12" t="n"/>
-      <c r="B48" s="13" t="n"/>
+      <c r="A48" s="7" t="n"/>
       <c r="C48" s="5" t="inlineStr">
         <is>
           <t>Paula Ferreira</t>
         </is>
       </c>
-      <c r="D48" s="10" t="n"/>
+      <c r="D48" s="7" t="n"/>
       <c r="E48" s="5" t="n">
         <v>6</v>
       </c>
@@ -4907,17 +3801,16 @@
       <c r="W48" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X48" s="14" t="n"/>
+      <c r="X48" s="7" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" s="12" t="n"/>
-      <c r="B49" s="13" t="n"/>
+      <c r="A49" s="7" t="n"/>
       <c r="C49" s="5" t="inlineStr">
         <is>
           <t>Paulo Vieira</t>
         </is>
       </c>
-      <c r="D49" s="10" t="n"/>
+      <c r="D49" s="7" t="n"/>
       <c r="E49" s="5" t="n">
         <v>5</v>
       </c>
@@ -4975,17 +3868,16 @@
       <c r="W49" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="X49" s="14" t="n"/>
+      <c r="X49" s="7" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" s="15" t="n"/>
-      <c r="B50" s="16" t="n"/>
+      <c r="A50" s="7" t="n"/>
       <c r="C50" s="5" t="inlineStr">
         <is>
           <t>Rafaela Carvalho</t>
         </is>
       </c>
-      <c r="D50" s="10" t="n"/>
+      <c r="D50" s="7" t="n"/>
       <c r="E50" s="5" t="n">
         <v>6</v>
       </c>
@@ -5043,7 +3935,7 @@
       <c r="W50" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="X50" s="17" t="n"/>
+      <c r="X50" s="7" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="5" t="inlineStr">
@@ -5051,13 +3943,13 @@
           <t>Gonçalo Figueiredo</t>
         </is>
       </c>
-      <c r="B51" s="11" t="n"/>
+      <c r="B51" s="7" t="n"/>
       <c r="C51" s="5" t="inlineStr">
         <is>
           <t>Catarina Milheiro</t>
         </is>
       </c>
-      <c r="D51" s="10" t="n"/>
+      <c r="D51" s="7" t="n"/>
       <c r="E51" s="5" t="n">
         <v>6</v>
       </c>
@@ -5122,14 +4014,13 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="12" t="n"/>
-      <c r="B52" s="13" t="n"/>
+      <c r="A52" s="7" t="n"/>
       <c r="C52" s="5" t="inlineStr">
         <is>
           <t>Goncalo Figueiredo</t>
         </is>
       </c>
-      <c r="D52" s="10" t="n"/>
+      <c r="D52" s="7" t="n"/>
       <c r="E52" s="5" t="n">
         <v>4</v>
       </c>
@@ -5187,17 +4078,16 @@
       <c r="W52" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X52" s="14" t="n"/>
+      <c r="X52" s="7" t="n"/>
     </row>
     <row r="53">
-      <c r="A53" s="12" t="n"/>
-      <c r="B53" s="13" t="n"/>
+      <c r="A53" s="7" t="n"/>
       <c r="C53" s="5" t="inlineStr">
         <is>
           <t>Ines Cabral</t>
         </is>
       </c>
-      <c r="D53" s="10" t="n"/>
+      <c r="D53" s="7" t="n"/>
       <c r="E53" s="5" t="n">
         <v>6</v>
       </c>
@@ -5255,17 +4145,16 @@
       <c r="W53" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X53" s="14" t="n"/>
+      <c r="X53" s="7" t="n"/>
     </row>
     <row r="54">
-      <c r="A54" s="12" t="n"/>
-      <c r="B54" s="13" t="n"/>
+      <c r="A54" s="7" t="n"/>
       <c r="C54" s="5" t="inlineStr">
         <is>
           <t>Mariana Arezes</t>
         </is>
       </c>
-      <c r="D54" s="10" t="n"/>
+      <c r="D54" s="7" t="n"/>
       <c r="E54" s="5" t="n">
         <v>6</v>
       </c>
@@ -5323,17 +4212,16 @@
       <c r="W54" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X54" s="14" t="n"/>
+      <c r="X54" s="7" t="n"/>
     </row>
     <row r="55">
-      <c r="A55" s="12" t="n"/>
-      <c r="B55" s="13" t="n"/>
+      <c r="A55" s="7" t="n"/>
       <c r="C55" s="5" t="inlineStr">
         <is>
           <t>Mariana Oliveira</t>
         </is>
       </c>
-      <c r="D55" s="10" t="n"/>
+      <c r="D55" s="7" t="n"/>
       <c r="E55" s="5" t="n">
         <v>6</v>
       </c>
@@ -5391,17 +4279,16 @@
       <c r="W55" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X55" s="14" t="n"/>
+      <c r="X55" s="7" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" s="12" t="n"/>
-      <c r="B56" s="13" t="n"/>
+      <c r="A56" s="7" t="n"/>
       <c r="C56" s="5" t="inlineStr">
         <is>
           <t>Paula Ferreira</t>
         </is>
       </c>
-      <c r="D56" s="10" t="n"/>
+      <c r="D56" s="7" t="n"/>
       <c r="E56" s="5" t="n">
         <v>6</v>
       </c>
@@ -5459,17 +4346,16 @@
       <c r="W56" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X56" s="14" t="n"/>
+      <c r="X56" s="7" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" s="12" t="n"/>
-      <c r="B57" s="13" t="n"/>
+      <c r="A57" s="7" t="n"/>
       <c r="C57" s="5" t="inlineStr">
         <is>
           <t>Paulo Vieira</t>
         </is>
       </c>
-      <c r="D57" s="10" t="n"/>
+      <c r="D57" s="7" t="n"/>
       <c r="E57" s="5" t="n">
         <v>6</v>
       </c>
@@ -5527,17 +4413,16 @@
       <c r="W57" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X57" s="14" t="n"/>
+      <c r="X57" s="7" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" s="15" t="n"/>
-      <c r="B58" s="16" t="n"/>
+      <c r="A58" s="7" t="n"/>
       <c r="C58" s="5" t="inlineStr">
         <is>
           <t>Rafaela Carvalho</t>
         </is>
       </c>
-      <c r="D58" s="10" t="n"/>
+      <c r="D58" s="7" t="n"/>
       <c r="E58" s="5" t="n">
         <v>6</v>
       </c>
@@ -5595,7 +4480,7 @@
       <c r="W58" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X58" s="17" t="n"/>
+      <c r="X58" s="7" t="n"/>
     </row>
     <row r="59">
       <c r="A59" s="5" t="inlineStr">
@@ -5603,13 +4488,13 @@
           <t>Catarina Milheiro</t>
         </is>
       </c>
-      <c r="B59" s="11" t="n"/>
+      <c r="B59" s="7" t="n"/>
       <c r="C59" s="5" t="inlineStr">
         <is>
           <t>Catarina Milheiro</t>
         </is>
       </c>
-      <c r="D59" s="10" t="n"/>
+      <c r="D59" s="7" t="n"/>
       <c r="E59" s="5" t="n">
         <v>6</v>
       </c>
@@ -5674,14 +4559,13 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="12" t="n"/>
-      <c r="B60" s="13" t="n"/>
+      <c r="A60" s="7" t="n"/>
       <c r="C60" s="5" t="inlineStr">
         <is>
           <t>Goncalo Figueiredo</t>
         </is>
       </c>
-      <c r="D60" s="10" t="n"/>
+      <c r="D60" s="7" t="n"/>
       <c r="E60" s="5" t="n">
         <v>4</v>
       </c>
@@ -5739,17 +4623,16 @@
       <c r="W60" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="X60" s="14" t="n"/>
+      <c r="X60" s="7" t="n"/>
     </row>
     <row r="61">
-      <c r="A61" s="12" t="n"/>
-      <c r="B61" s="13" t="n"/>
+      <c r="A61" s="7" t="n"/>
       <c r="C61" s="5" t="inlineStr">
         <is>
           <t>Ines Cabral</t>
         </is>
       </c>
-      <c r="D61" s="10" t="n"/>
+      <c r="D61" s="7" t="n"/>
       <c r="E61" s="5" t="n">
         <v>4</v>
       </c>
@@ -5807,17 +4690,16 @@
       <c r="W61" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="X61" s="14" t="n"/>
+      <c r="X61" s="7" t="n"/>
     </row>
     <row r="62">
-      <c r="A62" s="12" t="n"/>
-      <c r="B62" s="13" t="n"/>
+      <c r="A62" s="7" t="n"/>
       <c r="C62" s="5" t="inlineStr">
         <is>
           <t>Mariana Arezes</t>
         </is>
       </c>
-      <c r="D62" s="10" t="n"/>
+      <c r="D62" s="7" t="n"/>
       <c r="E62" s="5" t="n">
         <v>6</v>
       </c>
@@ -5875,17 +4757,16 @@
       <c r="W62" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X62" s="14" t="n"/>
+      <c r="X62" s="7" t="n"/>
     </row>
     <row r="63">
-      <c r="A63" s="12" t="n"/>
-      <c r="B63" s="13" t="n"/>
+      <c r="A63" s="7" t="n"/>
       <c r="C63" s="5" t="inlineStr">
         <is>
           <t>Mariana Oliveira</t>
         </is>
       </c>
-      <c r="D63" s="10" t="n"/>
+      <c r="D63" s="7" t="n"/>
       <c r="E63" s="5" t="n">
         <v>6</v>
       </c>
@@ -5943,17 +4824,16 @@
       <c r="W63" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X63" s="14" t="n"/>
+      <c r="X63" s="7" t="n"/>
     </row>
     <row r="64">
-      <c r="A64" s="12" t="n"/>
-      <c r="B64" s="13" t="n"/>
+      <c r="A64" s="7" t="n"/>
       <c r="C64" s="5" t="inlineStr">
         <is>
           <t>Paula Ferreira</t>
         </is>
       </c>
-      <c r="D64" s="10" t="n"/>
+      <c r="D64" s="7" t="n"/>
       <c r="E64" s="5" t="n">
         <v>6</v>
       </c>
@@ -6011,17 +4891,16 @@
       <c r="W64" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X64" s="14" t="n"/>
+      <c r="X64" s="7" t="n"/>
     </row>
     <row r="65">
-      <c r="A65" s="12" t="n"/>
-      <c r="B65" s="13" t="n"/>
+      <c r="A65" s="7" t="n"/>
       <c r="C65" s="5" t="inlineStr">
         <is>
           <t>Paulo Vieira</t>
         </is>
       </c>
-      <c r="D65" s="10" t="n"/>
+      <c r="D65" s="7" t="n"/>
       <c r="E65" s="5" t="n">
         <v>5</v>
       </c>
@@ -6079,17 +4958,16 @@
       <c r="W65" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X65" s="14" t="n"/>
+      <c r="X65" s="7" t="n"/>
     </row>
     <row r="66">
-      <c r="A66" s="15" t="n"/>
-      <c r="B66" s="16" t="n"/>
+      <c r="A66" s="7" t="n"/>
       <c r="C66" s="5" t="inlineStr">
         <is>
           <t>Rafaela Carvalho</t>
         </is>
       </c>
-      <c r="D66" s="10" t="n"/>
+      <c r="D66" s="7" t="n"/>
       <c r="E66" s="5" t="n">
         <v>4</v>
       </c>
@@ -6147,7 +5025,7 @@
       <c r="W66" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="X66" s="17" t="n"/>
+      <c r="X66" s="7" t="n"/>
     </row>
     <row r="67">
       <c r="A67" s="5" t="inlineStr">
@@ -6155,13 +5033,13 @@
           <t>Inês Bastos</t>
         </is>
       </c>
-      <c r="B67" s="11" t="n"/>
+      <c r="B67" s="7" t="n"/>
       <c r="C67" s="5" t="inlineStr">
         <is>
           <t>Catarina Milheiro</t>
         </is>
       </c>
-      <c r="D67" s="10" t="n"/>
+      <c r="D67" s="7" t="n"/>
       <c r="E67" s="5" t="n">
         <v>6</v>
       </c>
@@ -6226,14 +5104,13 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="12" t="n"/>
-      <c r="B68" s="13" t="n"/>
+      <c r="A68" s="7" t="n"/>
       <c r="C68" s="5" t="inlineStr">
         <is>
           <t>Goncalo Figueiredo</t>
         </is>
       </c>
-      <c r="D68" s="10" t="n"/>
+      <c r="D68" s="7" t="n"/>
       <c r="E68" s="5" t="n">
         <v>4</v>
       </c>
@@ -6291,17 +5168,16 @@
       <c r="W68" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X68" s="14" t="n"/>
+      <c r="X68" s="7" t="n"/>
     </row>
     <row r="69">
-      <c r="A69" s="12" t="n"/>
-      <c r="B69" s="13" t="n"/>
+      <c r="A69" s="7" t="n"/>
       <c r="C69" s="5" t="inlineStr">
         <is>
           <t>Ines Cabral</t>
         </is>
       </c>
-      <c r="D69" s="10" t="n"/>
+      <c r="D69" s="7" t="n"/>
       <c r="E69" s="5" t="n">
         <v>4</v>
       </c>
@@ -6359,17 +5235,16 @@
       <c r="W69" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X69" s="14" t="n"/>
+      <c r="X69" s="7" t="n"/>
     </row>
     <row r="70">
-      <c r="A70" s="12" t="n"/>
-      <c r="B70" s="13" t="n"/>
+      <c r="A70" s="7" t="n"/>
       <c r="C70" s="5" t="inlineStr">
         <is>
           <t>Mariana Arezes</t>
         </is>
       </c>
-      <c r="D70" s="10" t="n"/>
+      <c r="D70" s="7" t="n"/>
       <c r="E70" s="5" t="n">
         <v>6</v>
       </c>
@@ -6427,17 +5302,16 @@
       <c r="W70" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X70" s="14" t="n"/>
+      <c r="X70" s="7" t="n"/>
     </row>
     <row r="71">
-      <c r="A71" s="12" t="n"/>
-      <c r="B71" s="13" t="n"/>
+      <c r="A71" s="7" t="n"/>
       <c r="C71" s="5" t="inlineStr">
         <is>
           <t>Mariana Oliveira</t>
         </is>
       </c>
-      <c r="D71" s="10" t="n"/>
+      <c r="D71" s="7" t="n"/>
       <c r="E71" s="5" t="n">
         <v>6</v>
       </c>
@@ -6495,17 +5369,16 @@
       <c r="W71" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X71" s="14" t="n"/>
+      <c r="X71" s="7" t="n"/>
     </row>
     <row r="72">
-      <c r="A72" s="12" t="n"/>
-      <c r="B72" s="13" t="n"/>
+      <c r="A72" s="7" t="n"/>
       <c r="C72" s="5" t="inlineStr">
         <is>
           <t>Paula Ferreira</t>
         </is>
       </c>
-      <c r="D72" s="10" t="n"/>
+      <c r="D72" s="7" t="n"/>
       <c r="E72" s="5" t="n">
         <v>6</v>
       </c>
@@ -6563,17 +5436,16 @@
       <c r="W72" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X72" s="14" t="n"/>
+      <c r="X72" s="7" t="n"/>
     </row>
     <row r="73">
-      <c r="A73" s="12" t="n"/>
-      <c r="B73" s="13" t="n"/>
+      <c r="A73" s="7" t="n"/>
       <c r="C73" s="5" t="inlineStr">
         <is>
           <t>Paulo Vieira</t>
         </is>
       </c>
-      <c r="D73" s="10" t="n"/>
+      <c r="D73" s="7" t="n"/>
       <c r="E73" s="5" t="n">
         <v>5</v>
       </c>
@@ -6631,17 +5503,16 @@
       <c r="W73" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X73" s="14" t="n"/>
+      <c r="X73" s="7" t="n"/>
     </row>
     <row r="74">
-      <c r="A74" s="15" t="n"/>
-      <c r="B74" s="16" t="n"/>
+      <c r="A74" s="7" t="n"/>
       <c r="C74" s="5" t="inlineStr">
         <is>
           <t>Rafaela Carvalho</t>
         </is>
       </c>
-      <c r="D74" s="10" t="n"/>
+      <c r="D74" s="7" t="n"/>
       <c r="E74" s="5" t="n">
         <v>4</v>
       </c>
@@ -6699,7 +5570,7 @@
       <c r="W74" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X74" s="17" t="n"/>
+      <c r="X74" s="7" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1481">
@@ -7828,8 +6699,8 @@
     <mergeCell ref="E60"/>
     <mergeCell ref="M22"/>
     <mergeCell ref="O50"/>
+    <mergeCell ref="M15"/>
     <mergeCell ref="P16"/>
-    <mergeCell ref="M15"/>
     <mergeCell ref="W12"/>
     <mergeCell ref="L41"/>
     <mergeCell ref="F27"/>
@@ -8187,743 +7058,4 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:W9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="18" t="inlineStr">
-        <is>
-          <t>Avaliação Mensal</t>
-        </is>
-      </c>
-      <c r="B1" s="8" t="n"/>
-      <c r="C1" s="8" t="n"/>
-      <c r="D1" s="8" t="n"/>
-      <c r="E1" s="8" t="n"/>
-      <c r="F1" s="8" t="n"/>
-      <c r="G1" s="8" t="n"/>
-      <c r="H1" s="8" t="n"/>
-      <c r="I1" s="8" t="n"/>
-      <c r="J1" s="8" t="n"/>
-      <c r="K1" s="8" t="n"/>
-      <c r="L1" s="8" t="n"/>
-      <c r="M1" s="8" t="n"/>
-      <c r="N1" s="8" t="n"/>
-      <c r="O1" s="8" t="n"/>
-      <c r="P1" s="8" t="n"/>
-      <c r="Q1" s="8" t="n"/>
-      <c r="R1" s="8" t="n"/>
-      <c r="S1" s="9" t="n"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="19" t="inlineStr">
-        <is>
-          <t>1. O membro coopera com os seus colegas para alcançar objetivos comuns que tenham sido estabelecidos.</t>
-        </is>
-      </c>
-      <c r="B2" s="19" t="inlineStr">
-        <is>
-          <t>2. O membro assume, em regra, objetivos ambiciosos e exigentes, embora realistas, para si e para os seus colegas.</t>
-        </is>
-      </c>
-      <c r="C2" s="19" t="inlineStr">
-        <is>
-          <t>3. O membro compromete-se com os resultados a alcançar de acordo com os objetivos estratégicos do departamento e júnior empresa, e é persistente perante obstáculos e dificuldades.</t>
-        </is>
-      </c>
-      <c r="D2" s="19" t="inlineStr">
-        <is>
-          <t>4. O membro aceita correr riscos para atingir os resultados desejados e assume as responsabilidades pelo sucesso ou fracasso dos mesmos.</t>
-        </is>
-      </c>
-      <c r="E2" s="19" t="inlineStr">
-        <is>
-          <t>5. O membro tem noção do que é prioritário para uma tarefa, respondendo, em regra, prontamente nos momentos de pressão e urgência.</t>
-        </is>
-      </c>
-      <c r="F2" s="19" t="inlineStr">
-        <is>
-          <t>6. O membro procura desenvolver o seu conhecimento técnico nas áreas relevantes para o seu departamento ou projeto em que esteja envolvido, promovendo um autodesenvolvimento contínuo.</t>
-        </is>
-      </c>
-      <c r="G2" s="19" t="inlineStr">
-        <is>
-          <t>1. O membro é capaz planear e organizar de forma eficiente atividades recreativas e/ou formações internas, de forma a que tenham sucesso.</t>
-        </is>
-      </c>
-      <c r="H2" s="19" t="inlineStr">
-        <is>
-          <t>2. O membro consegue elaborar relatórios de avaliações, de questionários de satisfação, etc., de uma forma clara e eficaz.</t>
-        </is>
-      </c>
-      <c r="I2" s="19" t="inlineStr">
-        <is>
-          <t>3. O membro acompanha as suas tarefas individuais recorrentes (p.ex: aniversários, avaliação motivacional, newsletters, etc.) de forma a confirmar que está tudo sob controlo.</t>
-        </is>
-      </c>
-      <c r="J2" s="19" t="inlineStr">
-        <is>
-          <t>4. O membro exibe criatividade durante a elaboração de atividades recreativas, planeamento de Recrutamento e Retiro, iniciativas internas, etc.</t>
-        </is>
-      </c>
-      <c r="K2" s="19" t="inlineStr">
-        <is>
-          <t>5. O membro lida com conflitos internos de uma forma preponderada, tendo em mente o melhor interesse dos membros e a estabilidade da EPIC Júnior.</t>
-        </is>
-      </c>
-      <c r="L2" s="19" t="inlineStr">
-        <is>
-          <t>6. O membro motiva os outros membros a participarem nas atividades internas da EPIC Júnior, bem como nas externas, da JE ou de outras Júnior Empresas.</t>
-        </is>
-      </c>
-      <c r="M2" s="19" t="inlineStr">
-        <is>
-          <t>1. O membro sabe comportar-se de uma forma correta e adequada e de uma maneira profissional e respeitosa, em situações em que representa a EPIC Júnior.</t>
-        </is>
-      </c>
-      <c r="N2" s="19" t="inlineStr">
-        <is>
-          <t>2. O membro respeita os valores, os membros, as instalações e todos os recursos da EPIC Júnior.</t>
-        </is>
-      </c>
-      <c r="O2" s="19" t="inlineStr">
-        <is>
-          <t>1. O membro cumpre os objetivos das tarefas pelos quais é responsável.</t>
-        </is>
-      </c>
-      <c r="P2" s="19" t="inlineStr">
-        <is>
-          <t>2. O membro respeita o prazo de entrega das suas tarefas.</t>
-        </is>
-      </c>
-      <c r="Q2" s="19" t="inlineStr">
-        <is>
-          <t>3. O membro, caso necessário, desenvolve conhecimento técnico especifico para completar a sua tarefa.</t>
-        </is>
-      </c>
-      <c r="R2" s="19" t="inlineStr">
-        <is>
-          <t>4. Em tarefas de grupo, o membro é capaz de comunicar com os seus colegas de forma clara e concisa, conseguindo defender a sua opinião mas respeitando a opinião dos outros, mantendo uma boa relação interpessoal.</t>
-        </is>
-      </c>
-      <c r="S2" s="19" t="inlineStr">
-        <is>
-          <t>5. O membro é capaz de executar a sua tarefa de forma eficaz e com qualidade, apresentando espírito crítico, ou seja, questionando e analisando-a de forma racional.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "5.4", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "4.0", ""),IF(Avaliacao!A1="Ines Cabral", "4.5", ""),IF(Avaliacao!A1="Mariana Arezes", "5.1", ""),IF(Avaliacao!A1="Mariana Oliveira", "5.4", ""),IF(Avaliacao!A1="Paula Ferreira", "5.4", ""),IF(Avaliacao!A1="Paulo Vieira", "4.8", ""),IF(Avaliacao!A1="Rafaela Carvalho", "4.7", ""),IF(Avaliacao!A1="Pedro Machado", "-", ""),)</f>
-        <v/>
-      </c>
-      <c r="B3" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "5.3", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "3.6", ""),IF(Avaliacao!A1="Ines Cabral", "4.3", ""),IF(Avaliacao!A1="Mariana Arezes", "4.9", ""),IF(Avaliacao!A1="Mariana Oliveira", "5.2", ""),IF(Avaliacao!A1="Paula Ferreira", "5.2", ""),IF(Avaliacao!A1="Paulo Vieira", "4.6", ""),IF(Avaliacao!A1="Rafaela Carvalho", "4.6", ""),IF(Avaliacao!A1="Pedro Machado", "-", ""),)</f>
-        <v/>
-      </c>
-      <c r="C3" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "5.4", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "3.8", ""),IF(Avaliacao!A1="Ines Cabral", "4.6", ""),IF(Avaliacao!A1="Mariana Arezes", "5.1", ""),IF(Avaliacao!A1="Mariana Oliveira", "5.2", ""),IF(Avaliacao!A1="Paula Ferreira", "5.2", ""),IF(Avaliacao!A1="Paulo Vieira", "4.5", ""),IF(Avaliacao!A1="Rafaela Carvalho", "4.8", ""),IF(Avaliacao!A1="Pedro Machado", "-", ""),)</f>
-        <v/>
-      </c>
-      <c r="D3" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "5.3", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "4.1", ""),IF(Avaliacao!A1="Ines Cabral", "4.7", ""),IF(Avaliacao!A1="Mariana Arezes", "5.1", ""),IF(Avaliacao!A1="Mariana Oliveira", "5.3", ""),IF(Avaliacao!A1="Paula Ferreira", "5.3", ""),IF(Avaliacao!A1="Paulo Vieira", "4.9", ""),IF(Avaliacao!A1="Rafaela Carvalho", "4.8", ""),IF(Avaliacao!A1="Pedro Machado", "-", ""),)</f>
-        <v/>
-      </c>
-      <c r="E3" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "5.4", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "3.5", ""),IF(Avaliacao!A1="Ines Cabral", "4.4", ""),IF(Avaliacao!A1="Mariana Arezes", "5.0", ""),IF(Avaliacao!A1="Mariana Oliveira", "5.3", ""),IF(Avaliacao!A1="Paula Ferreira", "5.1", ""),IF(Avaliacao!A1="Paulo Vieira", "4.3", ""),IF(Avaliacao!A1="Rafaela Carvalho", "4.3", ""),IF(Avaliacao!A1="Pedro Machado", "-", ""),)</f>
-        <v/>
-      </c>
-      <c r="F3" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "5.3", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "4.2", ""),IF(Avaliacao!A1="Ines Cabral", "4.5", ""),IF(Avaliacao!A1="Mariana Arezes", "5.0", ""),IF(Avaliacao!A1="Mariana Oliveira", "5.1", ""),IF(Avaliacao!A1="Paula Ferreira", "4.9", ""),IF(Avaliacao!A1="Paulo Vieira", "4.8", ""),IF(Avaliacao!A1="Rafaela Carvalho", "4.7", ""),IF(Avaliacao!A1="Pedro Machado", "-", ""),)</f>
-        <v/>
-      </c>
-      <c r="G3" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "5.3", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "4.1", ""),IF(Avaliacao!A1="Ines Cabral", "4.5", ""),IF(Avaliacao!A1="Mariana Arezes", "4.9", ""),IF(Avaliacao!A1="Mariana Oliveira", "5.2", ""),IF(Avaliacao!A1="Paula Ferreira", "5.0", ""),IF(Avaliacao!A1="Paulo Vieira", "4.4", ""),IF(Avaliacao!A1="Rafaela Carvalho", "4.7", ""),IF(Avaliacao!A1="Pedro Machado", "-", ""),)</f>
-        <v/>
-      </c>
-      <c r="H3" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "5.4", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "4.1", ""),IF(Avaliacao!A1="Ines Cabral", "4.9", ""),IF(Avaliacao!A1="Mariana Arezes", "5.2", ""),IF(Avaliacao!A1="Mariana Oliveira", "5.3", ""),IF(Avaliacao!A1="Paula Ferreira", "5.2", ""),IF(Avaliacao!A1="Paulo Vieira", "4.5", ""),IF(Avaliacao!A1="Rafaela Carvalho", "4.8", ""),IF(Avaliacao!A1="Pedro Machado", "-", ""),)</f>
-        <v/>
-      </c>
-      <c r="I3" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "5.4", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "3.8", ""),IF(Avaliacao!A1="Ines Cabral", "4.6", ""),IF(Avaliacao!A1="Mariana Arezes", "4.9", ""),IF(Avaliacao!A1="Mariana Oliveira", "5.2", ""),IF(Avaliacao!A1="Paula Ferreira", "5.4", ""),IF(Avaliacao!A1="Paulo Vieira", "4.5", ""),IF(Avaliacao!A1="Rafaela Carvalho", "4.8", ""),IF(Avaliacao!A1="Pedro Machado", "-", ""),)</f>
-        <v/>
-      </c>
-      <c r="J3" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "4.9", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "4.6", ""),IF(Avaliacao!A1="Ines Cabral", "4.9", ""),IF(Avaliacao!A1="Mariana Arezes", "5.3", ""),IF(Avaliacao!A1="Mariana Oliveira", "5.1", ""),IF(Avaliacao!A1="Paula Ferreira", "5.1", ""),IF(Avaliacao!A1="Paulo Vieira", "5.1", ""),IF(Avaliacao!A1="Rafaela Carvalho", "5.0", ""),IF(Avaliacao!A1="Pedro Machado", "-", ""),)</f>
-        <v/>
-      </c>
-      <c r="K3" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "5.4", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "5.4", ""),IF(Avaliacao!A1="Ines Cabral", "5.3", ""),IF(Avaliacao!A1="Mariana Arezes", "5.4", ""),IF(Avaliacao!A1="Mariana Oliveira", "5.4", ""),IF(Avaliacao!A1="Paula Ferreira", "5.4", ""),IF(Avaliacao!A1="Paulo Vieira", "5.4", ""),IF(Avaliacao!A1="Rafaela Carvalho", "5.4", ""),IF(Avaliacao!A1="Pedro Machado", "-", ""),)</f>
-        <v/>
-      </c>
-      <c r="L3" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "4.8", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "4.0", ""),IF(Avaliacao!A1="Ines Cabral", "4.2", ""),IF(Avaliacao!A1="Mariana Arezes", "4.7", ""),IF(Avaliacao!A1="Mariana Oliveira", "4.7", ""),IF(Avaliacao!A1="Paula Ferreira", "4.5", ""),IF(Avaliacao!A1="Paulo Vieira", "4.2", ""),IF(Avaliacao!A1="Rafaela Carvalho", "4.3", ""),IF(Avaliacao!A1="Pedro Machado", "-", ""),)</f>
-        <v/>
-      </c>
-      <c r="M3" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "5.4", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "4.9", ""),IF(Avaliacao!A1="Ines Cabral", "5.0", ""),IF(Avaliacao!A1="Mariana Arezes", "5.3", ""),IF(Avaliacao!A1="Mariana Oliveira", "5.3", ""),IF(Avaliacao!A1="Paula Ferreira", "5.4", ""),IF(Avaliacao!A1="Paulo Vieira", "5.1", ""),IF(Avaliacao!A1="Rafaela Carvalho", "5.1", ""),IF(Avaliacao!A1="Pedro Machado", "-", ""),)</f>
-        <v/>
-      </c>
-      <c r="N3" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "5.4", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "5.2", ""),IF(Avaliacao!A1="Ines Cabral", "5.3", ""),IF(Avaliacao!A1="Mariana Arezes", "5.4", ""),IF(Avaliacao!A1="Mariana Oliveira", "5.4", ""),IF(Avaliacao!A1="Paula Ferreira", "5.4", ""),IF(Avaliacao!A1="Paulo Vieira", "5.4", ""),IF(Avaliacao!A1="Rafaela Carvalho", "5.3", ""),IF(Avaliacao!A1="Pedro Machado", "-", ""),)</f>
-        <v/>
-      </c>
-      <c r="O3" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "5.4", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "4.3", ""),IF(Avaliacao!A1="Ines Cabral", "4.9", ""),IF(Avaliacao!A1="Mariana Arezes", "5.1", ""),IF(Avaliacao!A1="Mariana Oliveira", "5.3", ""),IF(Avaliacao!A1="Paula Ferreira", "5.4", ""),IF(Avaliacao!A1="Paulo Vieira", "4.8", ""),IF(Avaliacao!A1="Rafaela Carvalho", "4.9", ""),IF(Avaliacao!A1="Pedro Machado", "-", ""),)</f>
-        <v/>
-      </c>
-      <c r="P3" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "5.3", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "3.9", ""),IF(Avaliacao!A1="Ines Cabral", "4.7", ""),IF(Avaliacao!A1="Mariana Arezes", "4.9", ""),IF(Avaliacao!A1="Mariana Oliveira", "5.2", ""),IF(Avaliacao!A1="Paula Ferreira", "5.3", ""),IF(Avaliacao!A1="Paulo Vieira", "4.7", ""),IF(Avaliacao!A1="Rafaela Carvalho", "4.8", ""),IF(Avaliacao!A1="Pedro Machado", "-", ""),)</f>
-        <v/>
-      </c>
-      <c r="Q3" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "5.2", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "4.6", ""),IF(Avaliacao!A1="Ines Cabral", "4.7", ""),IF(Avaliacao!A1="Mariana Arezes", "5.0", ""),IF(Avaliacao!A1="Mariana Oliveira", "5.2", ""),IF(Avaliacao!A1="Paula Ferreira", "4.9", ""),IF(Avaliacao!A1="Paulo Vieira", "5.0", ""),IF(Avaliacao!A1="Rafaela Carvalho", "4.7", ""),IF(Avaliacao!A1="Pedro Machado", "-", ""),)</f>
-        <v/>
-      </c>
-      <c r="R3" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "5.3", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "5.0", ""),IF(Avaliacao!A1="Ines Cabral", "4.9", ""),IF(Avaliacao!A1="Mariana Arezes", "5.3", ""),IF(Avaliacao!A1="Mariana Oliveira", "5.4", ""),IF(Avaliacao!A1="Paula Ferreira", "5.2", ""),IF(Avaliacao!A1="Paulo Vieira", "5.2", ""),IF(Avaliacao!A1="Rafaela Carvalho", "5.1", ""),IF(Avaliacao!A1="Pedro Machado", "-", ""),)</f>
-        <v/>
-      </c>
-      <c r="S3" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "5.4", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "4.2", ""),IF(Avaliacao!A1="Ines Cabral", "4.6", ""),IF(Avaliacao!A1="Mariana Arezes", "5.2", ""),IF(Avaliacao!A1="Mariana Oliveira", "5.3", ""),IF(Avaliacao!A1="Paula Ferreira", "5.4", ""),IF(Avaliacao!A1="Paulo Vieira", "5.0", ""),IF(Avaliacao!A1="Rafaela Carvalho", "4.7", ""),IF(Avaliacao!A1="Pedro Machado", "-", ""),)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "5.3", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "4.278947368421052", ""),IF(Avaliacao!A1="Ines Cabral", "4.710526315789474", ""),IF(Avaliacao!A1="Mariana Arezes", "5.094736842105264", ""),IF(Avaliacao!A1="Mariana Oliveira", "5.236842105263158", ""),IF(Avaliacao!A1="Paula Ferreira", "5.194736842105264", ""),IF(Avaliacao!A1="Paulo Vieira", "4.8", ""),IF(Avaliacao!A1="Rafaela Carvalho", "4.815789473684211", ""),IF(Avaliacao!A1="Pedro Machado", "0.0", ""),)</f>
-        <v/>
-      </c>
-      <c r="B4" s="8" t="n"/>
-      <c r="C4" s="8" t="n"/>
-      <c r="D4" s="8" t="n"/>
-      <c r="E4" s="8" t="n"/>
-      <c r="F4" s="8" t="n"/>
-      <c r="G4" s="8" t="n"/>
-      <c r="H4" s="8" t="n"/>
-      <c r="I4" s="8" t="n"/>
-      <c r="J4" s="8" t="n"/>
-      <c r="K4" s="8" t="n"/>
-      <c r="L4" s="8" t="n"/>
-      <c r="M4" s="8" t="n"/>
-      <c r="N4" s="8" t="n"/>
-      <c r="O4" s="8" t="n"/>
-      <c r="P4" s="8" t="n"/>
-      <c r="Q4" s="8" t="n"/>
-      <c r="R4" s="8" t="n"/>
-      <c r="S4" s="9" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="18" t="inlineStr">
-        <is>
-          <t>Avaliação Mensal</t>
-        </is>
-      </c>
-      <c r="B6" s="8" t="n"/>
-      <c r="C6" s="8" t="n"/>
-      <c r="D6" s="8" t="n"/>
-      <c r="E6" s="8" t="n"/>
-      <c r="F6" s="8" t="n"/>
-      <c r="G6" s="8" t="n"/>
-      <c r="H6" s="8" t="n"/>
-      <c r="I6" s="8" t="n"/>
-      <c r="J6" s="8" t="n"/>
-      <c r="K6" s="8" t="n"/>
-      <c r="L6" s="8" t="n"/>
-      <c r="M6" s="8" t="n"/>
-      <c r="N6" s="8" t="n"/>
-      <c r="O6" s="8" t="n"/>
-      <c r="P6" s="8" t="n"/>
-      <c r="Q6" s="8" t="n"/>
-      <c r="R6" s="8" t="n"/>
-      <c r="S6" s="8" t="n"/>
-      <c r="T6" s="8" t="n"/>
-      <c r="U6" s="8" t="n"/>
-      <c r="V6" s="8" t="n"/>
-      <c r="W6" s="9" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE coopera com os seus colegas para alcançar objetivos comuns que tenham sido estabelecidos.</t>
-        </is>
-      </c>
-      <c r="B7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE assume, em regra, objetivos ambiciosos e exigentes, embora realistas, para si e para os seus colegas.</t>
-        </is>
-      </c>
-      <c r="C7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE compromete-se com os resultados a alcançar de acordo com os objetivos estratégicos da júnior empresa, e é persistente perante obstáculos e dificuldades.</t>
-        </is>
-      </c>
-      <c r="D7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE aceita correr riscos para atingir os resultados desejados e assume as responsabilidades pelo sucesso ou fracasso dos mesmos.</t>
-        </is>
-      </c>
-      <c r="E7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE tem noção do que é prioritário para uma tarefa, respondendo, em regra, prontamente nos momentos de pressão e urgência.</t>
-        </is>
-      </c>
-      <c r="F7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE procura desenvolver o seu conhecimento técnico nas áreas relevantes para o seu departamento ou projeto em que esteja envolvido, promovendo um autodesenvolvimento contínuo.</t>
-        </is>
-      </c>
-      <c r="G7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE tem em conta as necessidades, requisitos e opiniões do cliente no desenvolvimento de um projeto.</t>
-        </is>
-      </c>
-      <c r="H7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE sabe delegar tarefas de forma produtiva, justa e homogénea. Consegue manter uma dinâmica de departamento saudável e tem como objetivo o trabalho em equipa.</t>
-        </is>
-      </c>
-      <c r="I7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE tenta obter o resultado mais vantajoso possível para os projetos e para a EPIC Júnior sem comprometer padrões éticos, senso comum e a confiança do cliente.</t>
-        </is>
-      </c>
-      <c r="J7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE sabe aproveitar ao máximo e integrar os recursos disponíveis dentro da EPIC Júnior, de forma global. Consegue reavaliar, aprimorar e padronizar os processos de trabalho.</t>
-        </is>
-      </c>
-      <c r="K7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE tem a capacidade de estabelecer uma rede de contactos ou uma conexão a empresas que possam ser futuros clientes.</t>
-        </is>
-      </c>
-      <c r="L7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE tem a capacidade de convencer pessoas, ou mudar a sua perspetiva, usando o seu poder de argumentação, raciocínio e lógica.</t>
-        </is>
-      </c>
-      <c r="M7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE consegue estruturar o seu pensamento de forma coerente, levando a boas conclusões. Sabe desenvolver estratégias ou ideias bem planeadas/estruturadas</t>
-        </is>
-      </c>
-      <c r="N7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE consegue organizar o que faz de forma eficiente e clara, exibindo uma boa gestão de tarefas e tempo.</t>
-        </is>
-      </c>
-      <c r="O7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE participa regularmente em formações internas e noutras atividades recreativas promovidas pelo departamento de Recursos Humanos.</t>
-        </is>
-      </c>
-      <c r="P7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE participa regularmente em reuniões gerais e reuniões de departamento.</t>
-        </is>
-      </c>
-      <c r="Q7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE sabe comportar-se de uma forma correta e adequada e de uma maneira profissional e respeitosa, em situações em que representa a EPIC Júnior.</t>
-        </is>
-      </c>
-      <c r="R7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE respeita os valores, os membros, as instalações e todos os recursos da EPIC Júnior.</t>
-        </is>
-      </c>
-      <c r="S7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE cumpre os objetivos das tarefas pelos quais é responsável.</t>
-        </is>
-      </c>
-      <c r="T7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE respeita o prazo de entrega das suas tarefas.</t>
-        </is>
-      </c>
-      <c r="U7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE, caso necessário, desenvolve conhecimento técnico especifico para completar a sua tarefa.</t>
-        </is>
-      </c>
-      <c r="V7" s="19" t="inlineStr">
-        <is>
-          <t>Em tarefas de grupo, o VPE é capaz de comunicar com os seus membros de forma clara e concisa, conseguindo defender a sua opinião mas respeitando a opinião dos outros, mantendo uma boa relação interpessoal.</t>
-        </is>
-      </c>
-      <c r="W7" s="19" t="inlineStr">
-        <is>
-          <t>O VPE é capaz de executar a sua tarefa de forma eficaz e com qualidade, apresentando espírito crítico, ou seja, questionando e analisando-a de forma racional.</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "5.142857142857143", ""),)</f>
-        <v/>
-      </c>
-      <c r="B8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "4.857142857142857", ""),)</f>
-        <v/>
-      </c>
-      <c r="C8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "5.142857142857143", ""),)</f>
-        <v/>
-      </c>
-      <c r="D8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "5.142857142857143", ""),)</f>
-        <v/>
-      </c>
-      <c r="E8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "4.714285714285714", ""),)</f>
-        <v/>
-      </c>
-      <c r="F8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "5.142857142857143", ""),)</f>
-        <v/>
-      </c>
-      <c r="G8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "5.142857142857143", ""),)</f>
-        <v/>
-      </c>
-      <c r="H8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "5.142857142857143", ""),)</f>
-        <v/>
-      </c>
-      <c r="I8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "5.0", ""),)</f>
-        <v/>
-      </c>
-      <c r="J8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "5.0", ""),)</f>
-        <v/>
-      </c>
-      <c r="K8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "5.0", ""),)</f>
-        <v/>
-      </c>
-      <c r="L8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "4.428571428571429", ""),)</f>
-        <v/>
-      </c>
-      <c r="M8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "4.857142857142857", ""),)</f>
-        <v/>
-      </c>
-      <c r="N8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "4.857142857142857", ""),)</f>
-        <v/>
-      </c>
-      <c r="O8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "5.0", ""),)</f>
-        <v/>
-      </c>
-      <c r="P8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "5.0", ""),)</f>
-        <v/>
-      </c>
-      <c r="Q8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "5.142857142857143", ""),)</f>
-        <v/>
-      </c>
-      <c r="R8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "5.0", ""),)</f>
-        <v/>
-      </c>
-      <c r="S8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "5.142857142857143", ""),)</f>
-        <v/>
-      </c>
-      <c r="T8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "4.857142857142857", ""),)</f>
-        <v/>
-      </c>
-      <c r="U8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "5.142857142857143", ""),)</f>
-        <v/>
-      </c>
-      <c r="V8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "4.857142857142857", ""),)</f>
-        <v/>
-      </c>
-      <c r="W8" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "-", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "-", ""),IF(Avaliacao!A1="Ines Cabral", "-", ""),IF(Avaliacao!A1="Mariana Arezes", "-", ""),IF(Avaliacao!A1="Mariana Oliveira", "-", ""),IF(Avaliacao!A1="Paula Ferreira", "-", ""),IF(Avaliacao!A1="Paulo Vieira", "-", ""),IF(Avaliacao!A1="Rafaela Carvalho", "-", ""),IF(Avaliacao!A1="Pedro Machado", "5.0", ""),)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="19">
-        <f>CONCATENAR(IF(Avaliacao!A1="Catarina Milheiro", "0.0", ""),IF(Avaliacao!A1="Goncalo Figueiredo", "0.0", ""),IF(Avaliacao!A1="Ines Cabral", "0.0", ""),IF(Avaliacao!A1="Mariana Arezes", "0.0", ""),IF(Avaliacao!A1="Mariana Oliveira", "0.0", ""),IF(Avaliacao!A1="Paula Ferreira", "0.0", ""),IF(Avaliacao!A1="Paulo Vieira", "0.0", ""),IF(Avaliacao!A1="Rafaela Carvalho", "0.0", ""),IF(Avaliacao!A1="Pedro Machado", "4.987577639751553", ""),)</f>
-        <v/>
-      </c>
-      <c r="B9" s="8" t="n"/>
-      <c r="C9" s="8" t="n"/>
-      <c r="D9" s="8" t="n"/>
-      <c r="E9" s="8" t="n"/>
-      <c r="F9" s="8" t="n"/>
-      <c r="G9" s="8" t="n"/>
-      <c r="H9" s="8" t="n"/>
-      <c r="I9" s="8" t="n"/>
-      <c r="J9" s="8" t="n"/>
-      <c r="K9" s="8" t="n"/>
-      <c r="L9" s="8" t="n"/>
-      <c r="M9" s="8" t="n"/>
-      <c r="N9" s="8" t="n"/>
-      <c r="O9" s="8" t="n"/>
-      <c r="P9" s="8" t="n"/>
-      <c r="Q9" s="8" t="n"/>
-      <c r="R9" s="8" t="n"/>
-      <c r="S9" s="8" t="n"/>
-      <c r="T9" s="8" t="n"/>
-      <c r="U9" s="8" t="n"/>
-      <c r="V9" s="8" t="n"/>
-      <c r="W9" s="9" t="n"/>
-    </row>
-  </sheetData>
-  <mergeCells count="88">
-    <mergeCell ref="I8"/>
-    <mergeCell ref="A9:W9"/>
-    <mergeCell ref="P3"/>
-    <mergeCell ref="C7"/>
-    <mergeCell ref="H3"/>
-    <mergeCell ref="J3"/>
-    <mergeCell ref="E7"/>
-    <mergeCell ref="G2"/>
-    <mergeCell ref="I2"/>
-    <mergeCell ref="S3"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="M2"/>
-    <mergeCell ref="P8"/>
-    <mergeCell ref="B8"/>
-    <mergeCell ref="L8"/>
-    <mergeCell ref="A3"/>
-    <mergeCell ref="N8"/>
-    <mergeCell ref="H7"/>
-    <mergeCell ref="J7"/>
-    <mergeCell ref="K8"/>
-    <mergeCell ref="R3"/>
-    <mergeCell ref="T8"/>
-    <mergeCell ref="D3"/>
-    <mergeCell ref="K7"/>
-    <mergeCell ref="R2"/>
-    <mergeCell ref="A4:S4"/>
-    <mergeCell ref="J2"/>
-    <mergeCell ref="O7"/>
-    <mergeCell ref="Q7"/>
-    <mergeCell ref="E8"/>
-    <mergeCell ref="G8"/>
-    <mergeCell ref="N3"/>
-    <mergeCell ref="Q8"/>
-    <mergeCell ref="F3"/>
-    <mergeCell ref="A7"/>
-    <mergeCell ref="S8"/>
-    <mergeCell ref="S2"/>
-    <mergeCell ref="G3"/>
-    <mergeCell ref="I3"/>
-    <mergeCell ref="D7"/>
-    <mergeCell ref="A2"/>
-    <mergeCell ref="C2"/>
-    <mergeCell ref="P7"/>
-    <mergeCell ref="E2"/>
-    <mergeCell ref="M3"/>
-    <mergeCell ref="T7"/>
-    <mergeCell ref="D8"/>
-    <mergeCell ref="V7"/>
-    <mergeCell ref="H8"/>
-    <mergeCell ref="J8"/>
-    <mergeCell ref="O3"/>
-    <mergeCell ref="A6:W6"/>
-    <mergeCell ref="Q3"/>
-    <mergeCell ref="L2"/>
-    <mergeCell ref="L3"/>
-    <mergeCell ref="G7"/>
-    <mergeCell ref="I7"/>
-    <mergeCell ref="P2"/>
-    <mergeCell ref="S7"/>
-    <mergeCell ref="M7"/>
-    <mergeCell ref="K2"/>
-    <mergeCell ref="A8"/>
-    <mergeCell ref="C8"/>
-    <mergeCell ref="U8"/>
-    <mergeCell ref="M8"/>
-    <mergeCell ref="W8"/>
-    <mergeCell ref="O8"/>
-    <mergeCell ref="O2"/>
-    <mergeCell ref="Q2"/>
-    <mergeCell ref="K3"/>
-    <mergeCell ref="C3"/>
-    <mergeCell ref="E3"/>
-    <mergeCell ref="R8"/>
-    <mergeCell ref="B7"/>
-    <mergeCell ref="L7"/>
-    <mergeCell ref="N7"/>
-    <mergeCell ref="B3"/>
-    <mergeCell ref="V8"/>
-    <mergeCell ref="F7"/>
-    <mergeCell ref="R7"/>
-    <mergeCell ref="B2"/>
-    <mergeCell ref="D2"/>
-    <mergeCell ref="N2"/>
-    <mergeCell ref="F8"/>
-    <mergeCell ref="F2"/>
-    <mergeCell ref="H2"/>
-    <mergeCell ref="U7"/>
-    <mergeCell ref="W7"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Catarina Milheiro</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Goncalo Figueiredo</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Ines Cabral</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Mariana Arezes</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Mariana Oliveira</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Paula Ferreira</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Paulo Vieira</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Rafaela Carvalho</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Pedro Machado</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="18">
-    <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=$B$1:$B$9</formula1>
-    </dataValidation>
-    <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=$B$1:$B$0</formula1>
-    </dataValidation>
-    <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=$B$1:$B$0</formula1>
-    </dataValidation>
-    <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=$B$1:$B$0</formula1>
-    </dataValidation>
-    <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=$B$1:$B$0</formula1>
-    </dataValidation>
-    <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=$B$1:$B$0</formula1>
-    </dataValidation>
-    <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=$B$1:$B$0</formula1>
-    </dataValidation>
-    <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=$B$1:$B$0</formula1>
-    </dataValidation>
-    <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=$B$1:$B$0</formula1>
-    </dataValidation>
-    <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=$B$1:$B$0</formula1>
-    </dataValidation>
-    <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=$B$1:$B$0</formula1>
-    </dataValidation>
-    <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=$B$1:$B$0</formula1>
-    </dataValidation>
-    <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=$B$1:$B$0</formula1>
-    </dataValidation>
-    <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=$B$1:$B$0</formula1>
-    </dataValidation>
-    <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=$B$1:$B$0</formula1>
-    </dataValidation>
-    <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=$B$1:$B$0</formula1>
-    </dataValidation>
-    <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=$B$1:$B$0</formula1>
-    </dataValidation>
-    <dataValidation sqref="A1" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=$B$1:$B$0</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>